<commit_message>
Optimus Counter Party Create Actions, TestData and other minor updates
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
+    <sheet name="CreateCounterParty" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
   <si>
     <t>Username</t>
   </si>
@@ -64,20 +65,305 @@
     <t>J6cxU20ke24l</t>
   </si>
   <si>
-    <t>QA_TestCase_Auto_Optimus_001</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_Optimus_002</t>
-  </si>
-  <si>
-    <t>QA_TestCase_Auto_Optimus_003</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>NitroClientID</t>
+  </si>
+  <si>
+    <t>SalesForceID</t>
+  </si>
+  <si>
+    <t>ElwoodID</t>
+  </si>
+  <si>
+    <t>NicknameExternal</t>
+  </si>
+  <si>
+    <t>NicknameInternal</t>
+  </si>
+  <si>
+    <t>ParentAccount</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
+    <t>CompanyofEmployment</t>
+  </si>
+  <si>
+    <t>IndustryofEmployment</t>
+  </si>
+  <si>
+    <t>IdentificationIssueDate/RegistrationDate</t>
+  </si>
+  <si>
+    <t>IdentificationExpiryDate</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>PEPDeclaration</t>
+  </si>
+  <si>
+    <t>PEPDeclaration/ScreeningRemarks</t>
+  </si>
+  <si>
+    <t>TIN1</t>
+  </si>
+  <si>
+    <t>TIN2</t>
+  </si>
+  <si>
+    <t>TIN3</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>FormerRegisteredName</t>
+  </si>
+  <si>
+    <t>ClientType</t>
+  </si>
+  <si>
+    <t>EntityType</t>
+  </si>
+  <si>
+    <t>IdentificationNumber</t>
+  </si>
+  <si>
+    <t>IdentificationType</t>
+  </si>
+  <si>
+    <t>RegisteredAddress</t>
+  </si>
+  <si>
+    <t>CountryofIncorporation/Residency</t>
+  </si>
+  <si>
+    <t>StateofIncorporation/Residency</t>
+  </si>
+  <si>
+    <t>OperatingAddress</t>
+  </si>
+  <si>
+    <t>CountryofOperation</t>
+  </si>
+  <si>
+    <t>OnboardingMode</t>
+  </si>
+  <si>
+    <t>PrimaryBusinessActivity</t>
+  </si>
+  <si>
+    <t>PrimaryBusinessActivityRemarks</t>
+  </si>
+  <si>
+    <t>CorporateWebsite</t>
+  </si>
+  <si>
+    <t>GSTRegistered</t>
+  </si>
+  <si>
+    <t>FinancialInstitution</t>
+  </si>
+  <si>
+    <t>PaymentServiceProvider</t>
+  </si>
+  <si>
+    <t>SourceofFunds</t>
+  </si>
+  <si>
+    <t>SourceofFundsRemarks</t>
+  </si>
+  <si>
+    <t>AuthorizedPerson</t>
+  </si>
+  <si>
+    <t>AuthorizedPersonMobile</t>
+  </si>
+  <si>
+    <t>AuthorizedPersonEmail</t>
+  </si>
+  <si>
+    <t>BusinessPurposeforRelationship</t>
+  </si>
+  <si>
+    <t>Appointment(Others)</t>
+  </si>
+  <si>
+    <t>GroupAssociation</t>
+  </si>
+  <si>
+    <t>OnboardedDate</t>
+  </si>
+  <si>
+    <t>ClientTier</t>
+  </si>
+  <si>
+    <t>KYCRefreshDate</t>
+  </si>
+  <si>
+    <t>ClientTierRemarks</t>
+  </si>
+  <si>
+    <t>RiskScore</t>
+  </si>
+  <si>
+    <t>RiskScoreRemarks</t>
+  </si>
+  <si>
+    <t>ExecutionFeeRate</t>
+  </si>
+  <si>
+    <t>ReferralPerson(Internal)</t>
+  </si>
+  <si>
+    <t>ReferralPerson(External)</t>
+  </si>
+  <si>
+    <t>ReferralExternalRebate</t>
+  </si>
+  <si>
+    <t>FacetoFaceVerificationStatus</t>
+  </si>
+  <si>
+    <t>FacetoFaceVerificationRemarks</t>
+  </si>
+  <si>
+    <t>VouchedStatus</t>
+  </si>
+  <si>
+    <t>VouchedbyPerson</t>
+  </si>
+  <si>
+    <t>VouchedRemarks</t>
+  </si>
+  <si>
+    <t>ManagementRemarks</t>
+  </si>
+  <si>
+    <t>CounterpartyStatus</t>
+  </si>
+  <si>
+    <t>CounterpartyRemarks</t>
+  </si>
+  <si>
+    <t>CounterparyRef</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_1_1</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_1_2</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_1_3</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_1_1</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_1_2</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_1_3</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_1_4</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_1_5</t>
+  </si>
+  <si>
+    <t>SalesForceIDAutomate1</t>
+  </si>
+  <si>
+    <t>SalesForceIDAutomate2</t>
+  </si>
+  <si>
+    <t>SalesForceIDAutomate3</t>
+  </si>
+  <si>
+    <t>SalesForceIDAutomate4</t>
+  </si>
+  <si>
+    <t>SalesForceIDAutomate5</t>
+  </si>
+  <si>
+    <t>NicknameInternalAutomate1</t>
+  </si>
+  <si>
+    <t>NicknameInternalAutomate2</t>
+  </si>
+  <si>
+    <t>NicknameInternalAutomate3</t>
+  </si>
+  <si>
+    <t>NicknameInternalAutomate4</t>
+  </si>
+  <si>
+    <t>NicknameInternalAutomate5</t>
+  </si>
+  <si>
+    <t>TIN1Test1</t>
+  </si>
+  <si>
+    <t>TIN1Test2</t>
+  </si>
+  <si>
+    <t>TIN1Test3</t>
+  </si>
+  <si>
+    <t>TIN1Test4</t>
+  </si>
+  <si>
+    <t>TIN1Test5</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Limited Company</t>
+  </si>
+  <si>
+    <t>RegisteredAddress Automate 1</t>
+  </si>
+  <si>
+    <t>RegisteredAddress Automate 2</t>
+  </si>
+  <si>
+    <t>RegisteredAddress Automate 3</t>
+  </si>
+  <si>
+    <t>RegisteredAddress Automate 4</t>
+  </si>
+  <si>
+    <t>RegisteredAddress Automate 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +377,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +394,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -138,11 +432,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,6 +490,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,7 +846,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -513,7 +864,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -531,7 +882,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -590,4 +941,414 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BQ6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="W4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="W5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF5" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Optimus Steps and Action
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456C886F-0E32-4F31-9FC4-DFBCAFB49C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -362,7 +363,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,6 +598,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -632,6 +650,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,7 +842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -934,9 +969,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -944,11 +979,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Optimus excel and added new sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456C886F-0E32-4F31-9FC4-DFBCAFB49C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA0CE0-E7E2-43F6-8720-C00000742416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
     <sheet name="CreateCounterParty" sheetId="11" r:id="rId2"/>
+    <sheet name="Settlement" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
   <si>
     <t>Username</t>
   </si>
@@ -358,6 +359,135 @@
   </si>
   <si>
     <t>RegisteredAddress Automate 5</t>
+  </si>
+  <si>
+    <t>Settlement Ref.</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>Counterparty Name</t>
+  </si>
+  <si>
+    <t>Counterparty ID</t>
+  </si>
+  <si>
+    <t>Settlement Nickname External</t>
+  </si>
+  <si>
+    <t>Settlement Nickname Internal</t>
+  </si>
+  <si>
+    <t>Settlement Type</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Currency Full Name</t>
+  </si>
+  <si>
+    <t>Transfer Method</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Custodian</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Bank Address</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>Bank Swift Code</t>
+  </si>
+  <si>
+    <t>Bank ABA Code</t>
+  </si>
+  <si>
+    <t>Bank Beneficiary Name</t>
+  </si>
+  <si>
+    <t>Bank Beneficiary Address</t>
+  </si>
+  <si>
+    <t>Bank Reference</t>
+  </si>
+  <si>
+    <t>Bank Remarks</t>
+  </si>
+  <si>
+    <t>Wallet Address</t>
+  </si>
+  <si>
+    <t>Wallet Memo</t>
+  </si>
+  <si>
+    <t>Wallet Remarks</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Whitelisting Method</t>
+  </si>
+  <si>
+    <t>Whitelisting Transfer Txid</t>
+  </si>
+  <si>
+    <t>Whitelisting Remarks</t>
+  </si>
+  <si>
+    <t>Settlement Status</t>
+  </si>
+  <si>
+    <t>Settlement Remarks</t>
+  </si>
+  <si>
+    <t>Bank Refs</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_3_1_1</t>
+  </si>
+  <si>
+    <t>Joejoe Pen</t>
+  </si>
+  <si>
+    <t>Joejoe - PNB - USD</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>SWIFT</t>
+  </si>
+  <si>
+    <t>DBS Singapore</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Trading</t>
   </si>
 </sst>
 </file>
@@ -982,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1386,4 +1516,188 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07C04E-058D-42DA-9D09-1E234291C2C3}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.81640625" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" t="s">
+        <v>132</v>
+      </c>
+      <c r="U1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V1" t="s">
+        <v>134</v>
+      </c>
+      <c r="W1" t="s">
+        <v>135</v>
+      </c>
+      <c r="X1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2">
+        <v>2710</v>
+      </c>
+      <c r="F2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" t="s">
+        <v>153</v>
+      </c>
+      <c r="W2">
+        <v>1434444</v>
+      </c>
+      <c r="X2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Optmized XAlpha and Optmius Added new test case 3_1_!
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA0CE0-E7E2-43F6-8720-C00000742416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CE72C2-BBA6-4518-A47F-05AF11005270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07C04E-058D-42DA-9D09-1E234291C2C3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1699,5 +1699,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Steps and Actions for New counter party
added ations, Refactor Main page name, update element locators, created step definitions, added test steps, added Test Data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CE72C2-BBA6-4518-A47F-05AF11005270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="175">
   <si>
     <t>Username</t>
   </si>
@@ -112,9 +111,6 @@
     <t>IndustryofEmployment</t>
   </si>
   <si>
-    <t>IdentificationIssueDate/RegistrationDate</t>
-  </si>
-  <si>
     <t>IdentificationExpiryDate</t>
   </si>
   <si>
@@ -157,12 +153,6 @@
     <t>RegisteredAddress</t>
   </si>
   <si>
-    <t>CountryofIncorporation/Residency</t>
-  </si>
-  <si>
-    <t>StateofIncorporation/Residency</t>
-  </si>
-  <si>
     <t>OperatingAddress</t>
   </si>
   <si>
@@ -235,12 +225,6 @@
     <t>ExecutionFeeRate</t>
   </si>
   <si>
-    <t>ReferralPerson(Internal)</t>
-  </si>
-  <si>
-    <t>ReferralPerson(External)</t>
-  </si>
-  <si>
     <t>ReferralExternalRebate</t>
   </si>
   <si>
@@ -488,13 +472,82 @@
   </si>
   <si>
     <t>Trading</t>
+  </si>
+  <si>
+    <t>IdentificationIssueDate</t>
+  </si>
+  <si>
+    <t>CountryofIncorporation</t>
+  </si>
+  <si>
+    <t>StateofIncorporation</t>
+  </si>
+  <si>
+    <t>ReferralPersonInternal</t>
+  </si>
+  <si>
+    <t>ReferralPersonExternal</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>QA_TEST_1</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Referral</t>
+  </si>
+  <si>
+    <t>Investments</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>joelan.pendon</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>QA_TEST_2</t>
+  </si>
+  <si>
+    <t>QA_TEST_3</t>
+  </si>
+  <si>
+    <t>QA_TEST_4</t>
+  </si>
+  <si>
+    <t>QA_TEST_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,14 +561,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -525,7 +570,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -608,11 +653,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -626,15 +682,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,23 +789,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -780,23 +824,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -972,7 +999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1011,7 +1038,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1029,7 +1056,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1047,7 +1074,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1099,9 +1126,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1109,407 +1136,666 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BQ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BR6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AV1" sqref="AV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1796875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="33.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="24.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="23.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="29.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="31.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="19.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="70" max="16384" width="40" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="BH1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="BI1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="BK1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BO1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR1" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA2" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD2" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP2" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AV1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AZ1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="BE1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="BF1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="BH1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="BJ1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="BL1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="BM1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="BN1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="BQ1" s="5" t="s">
-        <v>82</v>
+      <c r="D3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD3" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP3" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="W2" t="s">
+    <row r="4" spans="1:70" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG4" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH4" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD4" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG4" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM4" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP4" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF5" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AG5" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG5" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM5" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP5" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:70" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AF2" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="W3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="W4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF4" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="W5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF5" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:69" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="W6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>113</v>
+      <c r="AG6" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD6" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP6" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1519,10 +1805,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07C04E-058D-42DA-9D09-1E234291C2C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1545,97 +1831,97 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>118</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>119</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>120</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>121</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>122</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>123</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>124</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>125</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>126</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>127</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>128</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>129</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>130</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>131</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>132</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>133</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>134</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>135</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>136</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>137</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>138</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AF1" t="s">
         <v>139</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>144</v>
       </c>
       <c r="AG1" t="s">
         <v>11</v>
@@ -1646,49 +1932,49 @@
     </row>
     <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E2">
         <v>2710</v>
       </c>
       <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" t="s">
+        <v>146</v>
+      </c>
+      <c r="L2" t="s">
         <v>147</v>
       </c>
-      <c r="G2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="N2" t="s">
         <v>148</v>
-      </c>
-      <c r="I2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" t="s">
-        <v>152</v>
-      </c>
-      <c r="N2" t="s">
-        <v>153</v>
       </c>
       <c r="W2">
         <v>1434444</v>
       </c>
       <c r="X2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="Y2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Z2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AG2">
         <v>1</v>

</xml_diff>

<commit_message>
Update Optimus Excel Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="341">
   <si>
     <t>Username</t>
   </si>
@@ -120,9 +120,6 @@
     <t>PEPDeclaration</t>
   </si>
   <si>
-    <t>PEPDeclaration/ScreeningRemarks</t>
-  </si>
-  <si>
     <t>TIN1</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>BusinessPurposeforRelationship</t>
   </si>
   <si>
-    <t>Appointment(Others)</t>
-  </si>
-  <si>
     <t>GroupAssociation</t>
   </si>
   <si>
@@ -279,36 +273,6 @@
     <t>QA_TestCase_Auto_Optimus_2_1_5</t>
   </si>
   <si>
-    <t>SalesForceIDAutomate1</t>
-  </si>
-  <si>
-    <t>SalesForceIDAutomate2</t>
-  </si>
-  <si>
-    <t>SalesForceIDAutomate3</t>
-  </si>
-  <si>
-    <t>SalesForceIDAutomate4</t>
-  </si>
-  <si>
-    <t>SalesForceIDAutomate5</t>
-  </si>
-  <si>
-    <t>NicknameInternalAutomate1</t>
-  </si>
-  <si>
-    <t>NicknameInternalAutomate2</t>
-  </si>
-  <si>
-    <t>NicknameInternalAutomate3</t>
-  </si>
-  <si>
-    <t>NicknameInternalAutomate4</t>
-  </si>
-  <si>
-    <t>NicknameInternalAutomate5</t>
-  </si>
-  <si>
     <t>TIN1Test1</t>
   </si>
   <si>
@@ -553,13 +517,535 @@
   </si>
   <si>
     <t>new kingsway</t>
+  </si>
+  <si>
+    <t>SFIDTest1</t>
+  </si>
+  <si>
+    <t>SFIDTest2</t>
+  </si>
+  <si>
+    <t>SFIDTest3</t>
+  </si>
+  <si>
+    <t>SFIDTest4</t>
+  </si>
+  <si>
+    <t>SFIDTest5</t>
+  </si>
+  <si>
+    <t>NCIDTest1</t>
+  </si>
+  <si>
+    <t>NCIDTest2</t>
+  </si>
+  <si>
+    <t>NCIDTest3</t>
+  </si>
+  <si>
+    <t>NCIDTest4</t>
+  </si>
+  <si>
+    <t>NCIDTest5</t>
+  </si>
+  <si>
+    <t>EIDTest1</t>
+  </si>
+  <si>
+    <t>EIDTest2</t>
+  </si>
+  <si>
+    <t>EIDTest3</t>
+  </si>
+  <si>
+    <t>EIDTest4</t>
+  </si>
+  <si>
+    <t>EIDTest5</t>
+  </si>
+  <si>
+    <t>NickNameExt Test 1</t>
+  </si>
+  <si>
+    <t>NickNameExt Test 2</t>
+  </si>
+  <si>
+    <t>NickNameExt Test 3</t>
+  </si>
+  <si>
+    <t>NickNameExt Test 4</t>
+  </si>
+  <si>
+    <t>NickNameExt Test 5</t>
+  </si>
+  <si>
+    <t>NickName Int Test 2</t>
+  </si>
+  <si>
+    <t>NickName Int Test 3</t>
+  </si>
+  <si>
+    <t>NickName Int Test 4</t>
+  </si>
+  <si>
+    <t>NickName Int Test 5</t>
+  </si>
+  <si>
+    <t>NickName Int Test 6</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Automate 1</t>
+  </si>
+  <si>
+    <t>Automate 2</t>
+  </si>
+  <si>
+    <t>Automate 3</t>
+  </si>
+  <si>
+    <t>Automate 4</t>
+  </si>
+  <si>
+    <t>Automate 5</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>2000-01-01</t>
+  </si>
+  <si>
+    <t>Automation Test 1</t>
+  </si>
+  <si>
+    <t>Automation Test 2</t>
+  </si>
+  <si>
+    <t>Automation Test 3</t>
+  </si>
+  <si>
+    <t>Automation Test 4</t>
+  </si>
+  <si>
+    <t>Automation Test 5</t>
+  </si>
+  <si>
+    <t>2022-08-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2002-08-01 00:00:00</t>
+  </si>
+  <si>
+    <t>99887766554433</t>
+  </si>
+  <si>
+    <t>Toggle</t>
+  </si>
+  <si>
+    <t>PEP Declaration Screening Remarks Automate Test 1</t>
+  </si>
+  <si>
+    <t>PEP Declaration Screening Remarks Automate Test 2</t>
+  </si>
+  <si>
+    <t>PEP Declaration Screening Remarks Automate Test 3</t>
+  </si>
+  <si>
+    <t>PEP Declaration Screening Remarks Automate Test 4</t>
+  </si>
+  <si>
+    <t>PEP Declaration Screening Remarks Automate Test 5</t>
+  </si>
+  <si>
+    <t>Tin2Test1</t>
+  </si>
+  <si>
+    <t>Tin3Test1</t>
+  </si>
+  <si>
+    <t>Tin2Test2</t>
+  </si>
+  <si>
+    <t>Tin3Test2</t>
+  </si>
+  <si>
+    <t>Tin2Test3</t>
+  </si>
+  <si>
+    <t>Tin3Test3</t>
+  </si>
+  <si>
+    <t>Tin2Test4</t>
+  </si>
+  <si>
+    <t>Tin3Test4</t>
+  </si>
+  <si>
+    <t>Tin2Test5</t>
+  </si>
+  <si>
+    <t>Tin3Test5</t>
+  </si>
+  <si>
+    <t>TX Automate 1</t>
+  </si>
+  <si>
+    <t>TX Automate 2</t>
+  </si>
+  <si>
+    <t>TX Automate 3</t>
+  </si>
+  <si>
+    <t>TX Automate 4</t>
+  </si>
+  <si>
+    <t>TX Automate 5</t>
+  </si>
+  <si>
+    <t>TXA F Registered Name</t>
+  </si>
+  <si>
+    <t>IDNum1</t>
+  </si>
+  <si>
+    <t>IDNum2</t>
+  </si>
+  <si>
+    <t>IDNum3</t>
+  </si>
+  <si>
+    <t>IDNum4</t>
+  </si>
+  <si>
+    <t>IDNum5</t>
+  </si>
+  <si>
+    <t>TXA Primary Business Activity Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Primary Business Activity Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Primary Business Activity Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Primary Business Activity Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Primary Business Activity Remarks 5</t>
+  </si>
+  <si>
+    <t>www.CorporateWebsiteX.com</t>
+  </si>
+  <si>
+    <t>Https://www.CorporateWebsiteX.com</t>
+  </si>
+  <si>
+    <t>TXA Source of Funds Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Source of Funds Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Source of Funds Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Source of Funds Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Source of Funds Remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person 1</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Mobile 1</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Email 1</t>
+  </si>
+  <si>
+    <t>TXA Business Purpose for Relationship 1</t>
+  </si>
+  <si>
+    <t>TXA Appointment Others 1</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person 2</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Mobile 2</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Email 2</t>
+  </si>
+  <si>
+    <t>TXA Business Purpose for Relationship 2</t>
+  </si>
+  <si>
+    <t>TXA Appointment Others 2</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person 3</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Mobile 3</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Email 3</t>
+  </si>
+  <si>
+    <t>TXA Business Purpose for Relationship 3</t>
+  </si>
+  <si>
+    <t>TXA Appointment Others 3</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person 4</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Mobile 4</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Email 4</t>
+  </si>
+  <si>
+    <t>TXA Business Purpose for Relationship 4</t>
+  </si>
+  <si>
+    <t>TXA Appointment Others 4</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person 5</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Mobile 5</t>
+  </si>
+  <si>
+    <t>TXA Authorized Person Email 5</t>
+  </si>
+  <si>
+    <t>TXA Business Purpose for Relationship 5</t>
+  </si>
+  <si>
+    <t>TXA Appointment Others 5</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>TXA Group Association 1</t>
+  </si>
+  <si>
+    <t>TXA Group Association 2</t>
+  </si>
+  <si>
+    <t>TXA Group Association 3</t>
+  </si>
+  <si>
+    <t>TXA Group Association 4</t>
+  </si>
+  <si>
+    <t>TXA Group Association 5</t>
+  </si>
+  <si>
+    <t>TXA Client Tier remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Client Tier remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Client Tier remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Client Tier remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Client Tier remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Risk Score Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Risk Score Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Risk Score Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Risk Score Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Risk Score Remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Execution Fee Rate 1</t>
+  </si>
+  <si>
+    <t>TXA Execution Fee Rate 2</t>
+  </si>
+  <si>
+    <t>TXA Execution Fee Rate 3</t>
+  </si>
+  <si>
+    <t>TXA Execution Fee Rate 4</t>
+  </si>
+  <si>
+    <t>TXA Execution Fee Rate 5</t>
+  </si>
+  <si>
+    <t>amit.verma - -97</t>
+  </si>
+  <si>
+    <t>TXA Referral External Rebate 1</t>
+  </si>
+  <si>
+    <t>TXA Referral External Rebate 2</t>
+  </si>
+  <si>
+    <t>TXA Referral External Rebate 3</t>
+  </si>
+  <si>
+    <t>TXA Referral External Rebate 4</t>
+  </si>
+  <si>
+    <t>TXA Referral External Rebate 5</t>
+  </si>
+  <si>
+    <t>TXA FacetoFace Verification Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA FacetoFace Verification Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA FacetoFace Verification Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA FacetoFace Verification Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA FacetoFace Verification Remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Vouched Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Vouched Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Vouched Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Vouched Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Vouched Remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Management Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Management Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Management Remarks 5</t>
+  </si>
+  <si>
+    <t>TXA Management Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Management Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Counterparty Remarks 1</t>
+  </si>
+  <si>
+    <t>TXA Counterparty Remarks 2</t>
+  </si>
+  <si>
+    <t>TXA Counterparty Remarks 3</t>
+  </si>
+  <si>
+    <t>TXA Counterparty Remarks 4</t>
+  </si>
+  <si>
+    <t>TXA Counterparty Remarks 5</t>
+  </si>
+  <si>
+    <t>PEPDeclarationRemarks</t>
+  </si>
+  <si>
+    <t>AppointmentOthers</t>
+  </si>
+  <si>
+    <t>2022-12-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-12-01 00:00:01</t>
+  </si>
+  <si>
+    <t>2022-12-01 00:00:02</t>
+  </si>
+  <si>
+    <t>2022-12-01 00:00:03</t>
+  </si>
+  <si>
+    <t>2022-12-01 00:00:04</t>
+  </si>
+  <si>
+    <t>Txa Op Adr 1</t>
+  </si>
+  <si>
+    <t>Txa Op Adr 2</t>
+  </si>
+  <si>
+    <t>Txa Op Adr 3</t>
+  </si>
+  <si>
+    <t>Txa Op Adr 4</t>
+  </si>
+  <si>
+    <t>Txa Op Adr 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +1055,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -680,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -694,20 +1188,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,7 +1522,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,7 +1557,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1068,7 +1575,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1086,7 +1593,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1149,686 +1656,1387 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BT6"/>
+  <dimension ref="A1:BT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BS2" sqref="BS2"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="24.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="33.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="24.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="23.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="29.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="31.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="70" max="16384" width="40" style="9"/>
+    <col min="1" max="1" width="31.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="34.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="33.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="27.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="33.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="21.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="20.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="24.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="32.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="18.90625" style="7" customWidth="1"/>
+    <col min="71" max="71" width="13.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="5.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="73" max="16384" width="40" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="6" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AP1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AR1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AS1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AT1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AU1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AV1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AW1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AX1" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="AY1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="BA1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="BB1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BC1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BD1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BC1" s="6" t="s">
+      <c r="BE1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="BD1" s="6" t="s">
+      <c r="BF1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="BE1" s="6" t="s">
+      <c r="BG1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="BI1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="BF1" s="6" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="BG1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BH1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="BI1" s="6" t="s">
+      <c r="BK1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BJ1" s="6" t="s">
+      <c r="BL1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BK1" s="6" t="s">
+      <c r="BM1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BL1" s="6" t="s">
+      <c r="BN1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BM1" s="6" t="s">
+      <c r="BO1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BN1" s="6" t="s">
+      <c r="BP1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BO1" s="6" t="s">
+      <c r="BQ1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BP1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BQ1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BR1" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="BS1" t="s">
+      <c r="BR1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BS1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH2" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR2" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="BG2" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ2" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL2" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM2" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BP2" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="BS2"/>
-      <c r="BT2" t="b">
+    <row r="2" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH2" s="6"/>
+      <c r="BJ2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BM2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="14"/>
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE3" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH3" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK3" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR3" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA3" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD3" s="9" t="s">
+      <c r="A3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="BG3" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ3" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL3" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM3" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BP3" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT3" t="b">
+      <c r="E3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>250</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AZ3" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB3" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="BD3" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE3" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="BF3" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="BJ3" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK3" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="BL3" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN3" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="BO3" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="BP3" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ3" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="BS3" s="12"/>
+      <c r="BT3" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="A4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH4" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK4" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR4" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA4" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD4" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="BG4" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ4" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL4" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM4" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BP4" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT4" t="b">
+      <c r="I4" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD4" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG4" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>251</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS4" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AT4" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AU4" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="AV4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="AW4" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AX4" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="AY4" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="AZ4" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA4" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="BD4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE4" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="BF4" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI4" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="BJ4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK4" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="BL4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN4" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="BO4" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="BP4" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ4" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="BT4" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="A5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE5" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG5" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR5" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA5" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD5" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="BG5" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ5" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL5" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM5" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BP5" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT5" t="b">
+      <c r="AC5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="AE5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG5" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH5" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK5" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM5" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS5" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="AT5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AU5" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AV5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AW5" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="AX5" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AY5" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AZ5" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB5" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BD5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE5" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BF5" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI5" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="BJ5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK5" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="BL5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN5" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="BO5" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="BP5" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ5" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="BT5" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="A6" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="AD6" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG6" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH6" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS6" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="AT6" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="AU6" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="AV6" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="AW6" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AX6" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="AY6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="AZ6" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB6" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC6" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="BD6" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE6" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="BF6" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="BG6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH6" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI6" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="BJ6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK6" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="BL6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN6" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="BO6" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="BP6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ6" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="BT6" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE7" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC6" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE6" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG6" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH6" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR6" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA6" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD6" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="BG6" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ6" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL6" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM6" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BP6" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT6" t="b">
+      <c r="AG7" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH7" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI7" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK7" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM7" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>250</v>
+      </c>
+      <c r="AR7" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="AT7" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="AU7" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="AV7" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AW7" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AX7" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AZ7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA7" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC7" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="BD7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE7" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="BF7" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="BG7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BH7" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI7" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="BJ7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK7" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="BL7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN7" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="BO7" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="BP7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BQ7" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="BT7" s="12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1865,97 +3073,97 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" t="s">
+      <c r="O1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>113</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>114</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>116</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>117</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>118</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>119</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>120</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>121</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>122</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>123</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" t="s">
         <v>124</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>125</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>126</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>127</v>
-      </c>
-      <c r="U1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V1" t="s">
-        <v>129</v>
-      </c>
-      <c r="W1" t="s">
-        <v>130</v>
-      </c>
-      <c r="X1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>139</v>
       </c>
       <c r="AG1" t="s">
         <v>11</v>
@@ -1966,43 +3174,43 @@
     </row>
     <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E2">
         <v>2710</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="M2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="N2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="O2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="P2">
         <v>121212</v>
@@ -2011,22 +3219,22 @@
         <v>121</v>
       </c>
       <c r="S2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="T2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="W2">
         <v>1434444</v>
       </c>
       <c r="X2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="Y2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="Z2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="AG2">
         <v>1</v>

</xml_diff>

<commit_message>
Actions, Elements and steps for Test Case Creation 2_1_1
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B619C17-58C0-4DDC-8C01-A7D875007548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="340">
   <si>
     <t>Username</t>
   </si>
@@ -793,12 +792,6 @@
     <t>TXA Authorized Person 1</t>
   </si>
   <si>
-    <t>TXA Authorized Person Mobile 1</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person Email 1</t>
-  </si>
-  <si>
     <t>TXA Business Purpose for Relationship 1</t>
   </si>
   <si>
@@ -808,12 +801,6 @@
     <t>TXA Authorized Person 2</t>
   </si>
   <si>
-    <t>TXA Authorized Person Mobile 2</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person Email 2</t>
-  </si>
-  <si>
     <t>TXA Business Purpose for Relationship 2</t>
   </si>
   <si>
@@ -823,12 +810,6 @@
     <t>TXA Authorized Person 3</t>
   </si>
   <si>
-    <t>TXA Authorized Person Mobile 3</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person Email 3</t>
-  </si>
-  <si>
     <t>TXA Business Purpose for Relationship 3</t>
   </si>
   <si>
@@ -838,12 +819,6 @@
     <t>TXA Authorized Person 4</t>
   </si>
   <si>
-    <t>TXA Authorized Person Mobile 4</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person Email 4</t>
-  </si>
-  <si>
     <t>TXA Business Purpose for Relationship 4</t>
   </si>
   <si>
@@ -853,12 +828,6 @@
     <t>TXA Authorized Person 5</t>
   </si>
   <si>
-    <t>TXA Authorized Person Mobile 5</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person Email 5</t>
-  </si>
-  <si>
     <t>TXA Business Purpose for Relationship 5</t>
   </si>
   <si>
@@ -931,21 +900,6 @@
     <t>amit.verma - -97</t>
   </si>
   <si>
-    <t>TXA Referral External Rebate 1</t>
-  </si>
-  <si>
-    <t>TXA Referral External Rebate 2</t>
-  </si>
-  <si>
-    <t>TXA Referral External Rebate 3</t>
-  </si>
-  <si>
-    <t>TXA Referral External Rebate 4</t>
-  </si>
-  <si>
-    <t>TXA Referral External Rebate 5</t>
-  </si>
-  <si>
     <t>TXA FacetoFace Verification Remarks 1</t>
   </si>
   <si>
@@ -1058,12 +1012,36 @@
   </si>
   <si>
     <t>abb new value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>abc@abc.com</t>
+  </si>
+  <si>
+    <t>0998877665544</t>
+  </si>
+  <si>
+    <t>TXA Ref Ext Rebate 1</t>
+  </si>
+  <si>
+    <t>TXA Ref Ext Rebate 2</t>
+  </si>
+  <si>
+    <t>TXA Ref Ext Rebate 3</t>
+  </si>
+  <si>
+    <t>TXA Ref Ext Rebate 4</t>
+  </si>
+  <si>
+    <t>TXA Ref Ext Rebate 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1095,7 +1073,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1189,11 +1167,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1232,11 +1223,1639 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1247,6 +2866,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BT7" totalsRowShown="0" tableBorderDxfId="71">
+  <autoFilter ref="A1:BT7"/>
+  <tableColumns count="72">
+    <tableColumn id="1" name="TestCaseID" dataDxfId="70"/>
+    <tableColumn id="2" name="CounterparyRef" dataDxfId="69"/>
+    <tableColumn id="3" name="NitroClientID" dataDxfId="68"/>
+    <tableColumn id="4" name="SalesForceID" dataDxfId="67"/>
+    <tableColumn id="5" name="ElwoodID" dataDxfId="66"/>
+    <tableColumn id="6" name="NicknameExternal" dataDxfId="65"/>
+    <tableColumn id="7" name="NicknameInternal" dataDxfId="64"/>
+    <tableColumn id="8" name="ParentAccount" dataDxfId="63"/>
+    <tableColumn id="9" name="FirstName" dataDxfId="62"/>
+    <tableColumn id="10" name="LastName" dataDxfId="61"/>
+    <tableColumn id="11" name="Gender" dataDxfId="60"/>
+    <tableColumn id="12" name="Nationality" dataDxfId="59"/>
+    <tableColumn id="13" name="DateofBirth" dataDxfId="58"/>
+    <tableColumn id="14" name="Occupation" dataDxfId="57"/>
+    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="56"/>
+    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="55"/>
+    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="54"/>
+    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="53"/>
+    <tableColumn id="19" name="MobileNumber" dataDxfId="52"/>
+    <tableColumn id="20" name="PEPDeclaration" dataDxfId="51"/>
+    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="50"/>
+    <tableColumn id="22" name="Alias" dataDxfId="49"/>
+    <tableColumn id="23" name="TIN1" dataDxfId="48"/>
+    <tableColumn id="24" name="TIN2" dataDxfId="47"/>
+    <tableColumn id="25" name="TIN3" dataDxfId="46"/>
+    <tableColumn id="26" name="CompanyName" dataDxfId="45"/>
+    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="44"/>
+    <tableColumn id="28" name="ClientType" dataDxfId="43"/>
+    <tableColumn id="29" name="EntityType" dataDxfId="42"/>
+    <tableColumn id="30" name="IdentificationNumber" dataDxfId="41"/>
+    <tableColumn id="31" name="IdentificationType" dataDxfId="40"/>
+    <tableColumn id="32" name="RegisteredAddress" dataDxfId="39"/>
+    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="38"/>
+    <tableColumn id="34" name="StateofIncorporation" dataDxfId="37"/>
+    <tableColumn id="35" name="OperatingAddress" dataDxfId="36"/>
+    <tableColumn id="36" name="CountryofOperation" dataDxfId="35"/>
+    <tableColumn id="37" name="OnboardingMode" dataDxfId="34"/>
+    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="33"/>
+    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
+    <tableColumn id="40" name="CorporateWebsite"/>
+    <tableColumn id="41" name="GSTRegistered" dataDxfId="31"/>
+    <tableColumn id="42" name="FinancialInstitution" dataDxfId="30"/>
+    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="29"/>
+    <tableColumn id="44" name="SourceofFunds" dataDxfId="28"/>
+    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="27"/>
+    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="26"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="0"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="25"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="24"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="23"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="22"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="21"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="20"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="19"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="18"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="17"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="16"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="15"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="14"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="13"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="12"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="11"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="10"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="9"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="8"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="7"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="6"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="5"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="4"/>
+    <tableColumn id="70" name="Messages" dataDxfId="3"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="2"/>
+    <tableColumn id="72" name="SIT" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1325,23 +3025,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1377,23 +3060,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1569,7 +3235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1696,9 +3362,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1706,57 +3372,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT7"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3:BI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" style="6" customWidth="1"/>
     <col min="7" max="7" width="17.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="22.36328125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.453125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="21.7265625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="22.453125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="15.1796875" style="6" customWidth="1"/>
+    <col min="20" max="20" width="15.08984375" style="6" customWidth="1"/>
     <col min="21" max="21" width="44.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7265625" style="6" customWidth="1"/>
     <col min="23" max="23" width="9.08984375" style="6" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="8.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1796875" style="6" customWidth="1"/>
+    <col min="27" max="27" width="22.1796875" style="6" customWidth="1"/>
+    <col min="28" max="28" width="11.54296875" style="6" customWidth="1"/>
     <col min="29" max="29" width="15.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.36328125" style="6" customWidth="1"/>
+    <col min="31" max="31" width="17.6328125" style="6" customWidth="1"/>
     <col min="32" max="32" width="26.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.81640625" style="6" customWidth="1"/>
+    <col min="34" max="34" width="19.6328125" style="6" customWidth="1"/>
     <col min="35" max="35" width="21.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.08984375" style="6" customWidth="1"/>
+    <col min="37" max="37" width="17" style="6" customWidth="1"/>
+    <col min="38" max="38" width="22.1796875" style="6" customWidth="1"/>
     <col min="39" max="39" width="34.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="33.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.54296875" style="6" customWidth="1"/>
+    <col min="42" max="42" width="18.453125" style="6" customWidth="1"/>
+    <col min="43" max="43" width="22.7265625" style="6" customWidth="1"/>
+    <col min="44" max="44" width="14.81640625" style="6" customWidth="1"/>
     <col min="45" max="45" width="26.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="21" style="6" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="27.36328125" style="6" bestFit="1" customWidth="1"/>
@@ -1765,30 +3432,30 @@
     <col min="50" max="50" width="22.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="20.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.81640625" style="6" customWidth="1"/>
     <col min="54" max="54" width="17.81640625" style="6" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="21.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.54296875" style="6" customWidth="1"/>
     <col min="57" max="58" width="21.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="20.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="21.26953125" style="6" customWidth="1"/>
+    <col min="60" max="60" width="21.54296875" style="6" customWidth="1"/>
     <col min="61" max="61" width="25.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="24.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26.26953125" style="6" customWidth="1"/>
     <col min="63" max="63" width="32.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="19.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.90625" style="6" customWidth="1"/>
+    <col min="65" max="65" width="17.54296875" style="6" customWidth="1"/>
+    <col min="66" max="66" width="16.90625" style="6" customWidth="1"/>
+    <col min="67" max="67" width="20.36328125" style="6" customWidth="1"/>
+    <col min="68" max="68" width="18.453125" style="6" customWidth="1"/>
+    <col min="69" max="69" width="20.36328125" style="6" customWidth="1"/>
     <col min="70" max="70" width="18.90625" style="6" customWidth="1"/>
-    <col min="71" max="71" width="13.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.54296875" style="6" customWidth="1"/>
     <col min="72" max="72" width="5.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="73" max="16384" width="40" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -1849,7 +3516,7 @@
         <v>33</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>19</v>
@@ -1936,7 +3603,7 @@
         <v>58</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>59</v>
@@ -2006,7 +3673,7 @@
       </c>
     </row>
     <row r="2" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
@@ -2082,7 +3749,7 @@
       </c>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="5" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="BA2" s="12" t="s">
         <v>192</v>
@@ -2115,13 +3782,15 @@
       </c>
       <c r="BQ2" s="4"/>
       <c r="BR2" s="13"/>
-      <c r="BS2" s="11"/>
+      <c r="BS2" s="11" t="s">
+        <v>332</v>
+      </c>
       <c r="BT2" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="16" t="s">
         <v>80</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -2170,7 +3839,7 @@
         <v>216</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>217</v>
@@ -2215,7 +3884,7 @@
         <v>151</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="AJ3" s="6" t="s">
         <v>150</v>
@@ -2242,19 +3911,19 @@
         <v>257</v>
       </c>
       <c r="AU3" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AW3" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AX3" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="AW3" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="AX3" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="AY3" s="4" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="AZ3" s="6" t="s">
         <v>215</v>
@@ -2266,31 +3935,31 @@
         <v>215</v>
       </c>
       <c r="BC3" s="6" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="BD3" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE3" s="4" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BF3" s="4" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="BG3" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH3" s="6" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BI3" s="4" t="s">
-        <v>304</v>
+        <v>335</v>
       </c>
       <c r="BJ3" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK3" s="4" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="BL3" s="6" t="s">
         <v>157</v>
@@ -2299,24 +3968,26 @@
         <v>156</v>
       </c>
       <c r="BN3" s="4" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="BO3" s="4" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="BP3" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ3" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="BS3" s="11"/>
+        <v>309</v>
+      </c>
+      <c r="BS3" s="11" t="s">
+        <v>332</v>
+      </c>
       <c r="BT3" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -2365,7 +4036,7 @@
         <v>216</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>217</v>
@@ -2410,7 +4081,7 @@
         <v>151</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="AJ4" s="6" t="s">
         <v>150</v>
@@ -2434,22 +4105,22 @@
         <v>253</v>
       </c>
       <c r="AT4" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AW4" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="AX4" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="AU4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="AY4" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="AZ4" s="6" t="s">
         <v>215</v>
@@ -2461,31 +4132,31 @@
         <v>215</v>
       </c>
       <c r="BC4" s="6" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="BD4" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE4" s="4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="BF4" s="4" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="BG4" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH4" s="6" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BI4" s="4" t="s">
-        <v>305</v>
+        <v>336</v>
       </c>
       <c r="BJ4" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK4" s="4" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="BL4" s="6" t="s">
         <v>157</v>
@@ -2494,23 +4165,26 @@
         <v>156</v>
       </c>
       <c r="BN4" s="4" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="BO4" s="4" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="BP4" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ4" s="4" t="s">
-        <v>325</v>
+        <v>310</v>
+      </c>
+      <c r="BS4" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="BT4" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="16" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2559,7 +4233,7 @@
         <v>216</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>217</v>
@@ -2604,7 +4278,7 @@
         <v>151</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="AJ5" s="6" t="s">
         <v>150</v>
@@ -2628,22 +4302,22 @@
         <v>254</v>
       </c>
       <c r="AT5" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="AU5" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>269</v>
+        <v>334</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>333</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="AZ5" s="6" t="s">
         <v>215</v>
@@ -2655,31 +4329,31 @@
         <v>215</v>
       </c>
       <c r="BC5" s="6" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="BD5" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE5" s="4" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="BF5" s="4" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="BG5" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH5" s="6" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BI5" s="4" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="BJ5" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="BL5" s="6" t="s">
         <v>157</v>
@@ -2688,23 +4362,26 @@
         <v>156</v>
       </c>
       <c r="BN5" s="4" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="BO5" s="4" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="BP5" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>326</v>
+        <v>311</v>
+      </c>
+      <c r="BS5" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="BT5" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="16" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2753,7 +4430,7 @@
         <v>216</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>217</v>
@@ -2798,7 +4475,7 @@
         <v>151</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="AJ6" s="6" t="s">
         <v>150</v>
@@ -2822,22 +4499,22 @@
         <v>255</v>
       </c>
       <c r="AT6" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="AV6" s="4" t="s">
-        <v>274</v>
+        <v>334</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>333</v>
       </c>
       <c r="AW6" s="4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="AX6" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="AY6" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="AY6" s="4" t="s">
-        <v>286</v>
       </c>
       <c r="AZ6" s="6" t="s">
         <v>215</v>
@@ -2849,31 +4526,31 @@
         <v>215</v>
       </c>
       <c r="BC6" s="6" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="BD6" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE6" s="4" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="BF6" s="4" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="BG6" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH6" s="6" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BI6" s="4" t="s">
-        <v>307</v>
+        <v>338</v>
       </c>
       <c r="BJ6" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK6" s="4" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="BL6" s="6" t="s">
         <v>157</v>
@@ -2882,23 +4559,26 @@
         <v>156</v>
       </c>
       <c r="BN6" s="4" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="BO6" s="4" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="BP6" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ6" s="4" t="s">
-        <v>327</v>
+        <v>312</v>
+      </c>
+      <c r="BS6" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="BT6" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:72" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="16" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -2947,7 +4627,7 @@
         <v>216</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>217</v>
@@ -2992,7 +4672,7 @@
         <v>151</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AJ7" s="6" t="s">
         <v>150</v>
@@ -3016,22 +4696,22 @@
         <v>256</v>
       </c>
       <c r="AT7" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="AU7" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>333</v>
+      </c>
+      <c r="AW7" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AX7" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="AY7" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="AU7" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="AV7" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AW7" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="AX7" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="AY7" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="AZ7" s="6" t="s">
         <v>215</v>
@@ -3043,31 +4723,31 @@
         <v>215</v>
       </c>
       <c r="BC7" s="6" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="BD7" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE7" s="4" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="BF7" s="4" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="BG7" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH7" s="6" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BI7" s="4" t="s">
-        <v>308</v>
+        <v>339</v>
       </c>
       <c r="BJ7" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="BL7" s="6" t="s">
         <v>157</v>
@@ -3076,16 +4756,19 @@
         <v>156</v>
       </c>
       <c r="BN7" s="4" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="BO7" s="4" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="BP7" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ7" s="4" t="s">
-        <v>328</v>
+        <v>313</v>
+      </c>
+      <c r="BS7" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="BT7" s="11" t="b">
         <v>0</v>
@@ -3094,14 +4777,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3139,13 +4825,13 @@
         <v>101</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>102</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>103</v>
@@ -3246,7 +4932,7 @@
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
@@ -3315,7 +5001,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -3329,13 +5015,13 @@
         <v>130</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
added Test Case 2 1 1
Added Actions, Steps, Locators, Test Steps for MO and List pages.
Completed Test case 2_1_1
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="339">
   <si>
     <t>Username</t>
   </si>
@@ -534,21 +534,6 @@
     <t>SFIDTest5</t>
   </si>
   <si>
-    <t>NCIDTest1</t>
-  </si>
-  <si>
-    <t>NCIDTest2</t>
-  </si>
-  <si>
-    <t>NCIDTest3</t>
-  </si>
-  <si>
-    <t>NCIDTest4</t>
-  </si>
-  <si>
-    <t>NCIDTest5</t>
-  </si>
-  <si>
     <t>EIDTest1</t>
   </si>
   <si>
@@ -579,21 +564,6 @@
     <t>NickNameExt Test 5</t>
   </si>
   <si>
-    <t>NickName Int Test 2</t>
-  </si>
-  <si>
-    <t>NickName Int Test 3</t>
-  </si>
-  <si>
-    <t>NickName Int Test 4</t>
-  </si>
-  <si>
-    <t>NickName Int Test 5</t>
-  </si>
-  <si>
-    <t>NickName Int Test 6</t>
-  </si>
-  <si>
     <t>Dropdown</t>
   </si>
   <si>
@@ -1036,6 +1006,33 @@
   </si>
   <si>
     <t>TXA Ref Ext Rebate 5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>NNameIntTXA2</t>
+  </si>
+  <si>
+    <t>NNameIntTXA3</t>
+  </si>
+  <si>
+    <t>NNameIntTXA4</t>
+  </si>
+  <si>
+    <t>NNameIntTXA5</t>
+  </si>
+  <si>
+    <t>NNameIntTXA6</t>
   </si>
 </sst>
 </file>
@@ -1232,6 +1229,30 @@
   </cellStyles>
   <dxfs count="72">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1267,12 +1288,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1342,24 +1357,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1395,6 +1392,42 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1448,24 +1481,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1519,6 +1534,24 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1554,42 +1587,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1625,6 +1622,96 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1642,96 +1729,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -2918,32 +2915,32 @@
     <tableColumn id="44" name="SourceofFunds" dataDxfId="28"/>
     <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="27"/>
     <tableColumn id="46" name="AuthorizedPerson" dataDxfId="26"/>
-    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="0"/>
-    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="25"/>
-    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="24"/>
-    <tableColumn id="50" name="AppointmentOthers" dataDxfId="23"/>
-    <tableColumn id="51" name="GroupAssociation" dataDxfId="22"/>
-    <tableColumn id="52" name="OnboardedDate" dataDxfId="21"/>
-    <tableColumn id="53" name="ClientTier" dataDxfId="20"/>
-    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="19"/>
-    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="18"/>
-    <tableColumn id="56" name="RiskScore" dataDxfId="17"/>
-    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="16"/>
-    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="15"/>
-    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="14"/>
-    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="13"/>
-    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="12"/>
-    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="11"/>
-    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="10"/>
-    <tableColumn id="64" name="VouchedStatus" dataDxfId="9"/>
-    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="8"/>
-    <tableColumn id="66" name="VouchedRemarks" dataDxfId="7"/>
-    <tableColumn id="67" name="ManagementRemarks" dataDxfId="6"/>
-    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="5"/>
-    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="4"/>
-    <tableColumn id="70" name="Messages" dataDxfId="3"/>
-    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="2"/>
-    <tableColumn id="72" name="SIT" dataDxfId="1"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="25"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="24"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="23"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="22"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="21"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="20"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="19"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="18"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="17"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="16"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="15"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="14"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="13"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="12"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="11"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="8"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="7"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="6"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="5"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="4"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="3"/>
+    <tableColumn id="70" name="Messages" dataDxfId="2"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="72" name="SIT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3375,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BI3" sqref="BI3:BI7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3516,7 +3513,7 @@
         <v>33</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>19</v>
@@ -3603,7 +3600,7 @@
         <v>58</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>59</v>
@@ -3681,7 +3678,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3689,17 +3686,17 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -3709,81 +3706,81 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AD2" s="5"/>
       <c r="AE2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AH2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AL2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="AR2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="5" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="BA2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BB2" s="5"/>
       <c r="BC2" s="5"/>
       <c r="BD2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
       <c r="BG2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BH2" s="5"/>
       <c r="BJ2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BK2" s="4"/>
       <c r="BL2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BN2" s="4"/>
       <c r="BO2" s="4"/>
       <c r="BP2" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="BQ2" s="4"/>
       <c r="BR2" s="13"/>
       <c r="BS2" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT2" s="11" t="b">
         <v>0</v>
@@ -3794,73 +3791,73 @@
         <v>80</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>172</v>
+        <v>322</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>167</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>182</v>
-      </c>
       <c r="G3" s="14" t="s">
-        <v>187</v>
+        <v>334</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>146</v>
       </c>
       <c r="I3" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>203</v>
-      </c>
       <c r="L3" s="14" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>147</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>148</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>85</v>
       </c>
       <c r="X3" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z3" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="AA3" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="AB3" s="4" t="s">
         <v>90</v>
@@ -3869,7 +3866,7 @@
         <v>91</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="AE3" s="6" t="s">
         <v>149</v>
@@ -3884,7 +3881,7 @@
         <v>151</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="AJ3" s="6" t="s">
         <v>150</v>
@@ -3896,70 +3893,70 @@
         <v>148</v>
       </c>
       <c r="AM3" s="6" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="AN3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AR3" s="6" t="s">
         <v>153</v>
       </c>
       <c r="AS3" s="4" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="AU3" s="4" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="AV3" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="AW3" s="4" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="AX3" s="4" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="AY3" s="4" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="AZ3" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BA3" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BB3" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BC3" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="BD3" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE3" s="4" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="BF3" s="4" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="BG3" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH3" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BI3" s="4" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="BJ3" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK3" s="4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="BL3" s="6" t="s">
         <v>157</v>
@@ -3968,19 +3965,19 @@
         <v>156</v>
       </c>
       <c r="BN3" s="4" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="BO3" s="4" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="BP3" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ3" s="4" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="BS3" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT3" s="11" t="b">
         <v>0</v>
@@ -3991,73 +3988,73 @@
         <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>173</v>
+        <v>330</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>168</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>183</v>
-      </c>
       <c r="G4" s="14" t="s">
-        <v>188</v>
+        <v>335</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>159</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="L4" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>147</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>148</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>86</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="AB4" s="4" t="s">
         <v>90</v>
@@ -4066,7 +4063,7 @@
         <v>91</v>
       </c>
       <c r="AD4" s="6" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="AE4" s="6" t="s">
         <v>149</v>
@@ -4081,7 +4078,7 @@
         <v>151</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="AJ4" s="6" t="s">
         <v>150</v>
@@ -4093,70 +4090,70 @@
         <v>148</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="AN4" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="AR4" s="6" t="s">
         <v>153</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="AV4" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="AX4" s="4" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="AY4" s="4" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="AZ4" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BA4" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BB4" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BC4" s="6" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="BD4" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE4" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="BF4" s="4" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="BG4" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH4" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BI4" s="4" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="BJ4" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK4" s="4" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="BL4" s="6" t="s">
         <v>157</v>
@@ -4165,19 +4162,19 @@
         <v>156</v>
       </c>
       <c r="BN4" s="4" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="BO4" s="4" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="BP4" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ4" s="4" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="BS4" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT4" s="11" t="b">
         <v>0</v>
@@ -4188,73 +4185,73 @@
         <v>82</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>174</v>
+        <v>331</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>169</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>184</v>
-      </c>
       <c r="G5" s="14" t="s">
-        <v>189</v>
+        <v>336</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>160</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>147</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>148</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>87</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="Y5" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA5" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>90</v>
@@ -4263,7 +4260,7 @@
         <v>91</v>
       </c>
       <c r="AD5" s="6" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="AE5" s="6" t="s">
         <v>149</v>
@@ -4278,7 +4275,7 @@
         <v>151</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="AJ5" s="6" t="s">
         <v>150</v>
@@ -4290,70 +4287,70 @@
         <v>148</v>
       </c>
       <c r="AM5" s="6" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="AN5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AR5" s="6" t="s">
         <v>153</v>
       </c>
       <c r="AS5" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>323</v>
+      </c>
+      <c r="AW5" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="AT5" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>333</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="AX5" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AY5" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="AY5" s="4" t="s">
-        <v>275</v>
-      </c>
       <c r="AZ5" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BA5" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BB5" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BC5" s="6" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="BD5" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE5" s="4" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="BF5" s="4" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="BG5" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH5" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BI5" s="4" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="BJ5" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="BL5" s="6" t="s">
         <v>157</v>
@@ -4362,19 +4359,19 @@
         <v>156</v>
       </c>
       <c r="BN5" s="4" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="BO5" s="4" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="BP5" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="BS5" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT5" s="11" t="b">
         <v>0</v>
@@ -4385,73 +4382,73 @@
         <v>83</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>175</v>
+        <v>332</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>170</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>185</v>
-      </c>
       <c r="G6" s="14" t="s">
-        <v>190</v>
+        <v>337</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>161</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>147</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>148</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>88</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="AB6" s="4" t="s">
         <v>90</v>
@@ -4460,7 +4457,7 @@
         <v>91</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>149</v>
@@ -4475,7 +4472,7 @@
         <v>151</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="AJ6" s="6" t="s">
         <v>150</v>
@@ -4487,70 +4484,70 @@
         <v>148</v>
       </c>
       <c r="AM6" s="6" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="AN6" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="AR6" s="6" t="s">
         <v>153</v>
       </c>
       <c r="AS6" s="4" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="AT6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AW6" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="AY6" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="AU6" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>333</v>
-      </c>
-      <c r="AW6" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="AX6" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="AY6" s="4" t="s">
-        <v>276</v>
-      </c>
       <c r="AZ6" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BA6" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BB6" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BC6" s="6" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="BD6" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE6" s="4" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="BF6" s="4" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="BG6" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH6" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BI6" s="4" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="BJ6" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK6" s="4" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="BL6" s="6" t="s">
         <v>157</v>
@@ -4559,19 +4556,19 @@
         <v>156</v>
       </c>
       <c r="BN6" s="4" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="BO6" s="4" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="BP6" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ6" s="4" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="BS6" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT6" s="11" t="b">
         <v>0</v>
@@ -4582,73 +4579,73 @@
         <v>84</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>176</v>
+        <v>333</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>171</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>186</v>
-      </c>
       <c r="G7" s="14" t="s">
-        <v>191</v>
+        <v>338</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>162</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>147</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>148</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>89</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="AB7" s="4" t="s">
         <v>90</v>
@@ -4657,7 +4654,7 @@
         <v>91</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="AE7" s="6" t="s">
         <v>149</v>
@@ -4672,7 +4669,7 @@
         <v>151</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="AJ7" s="6" t="s">
         <v>150</v>
@@ -4684,70 +4681,70 @@
         <v>148</v>
       </c>
       <c r="AM7" s="6" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="AN7" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AR7" s="6" t="s">
         <v>153</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="AU7" s="4" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="AV7" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="AW7" s="4" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="AX7" s="4" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="AY7" s="4" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="AZ7" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BA7" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BB7" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="BC7" s="6" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="BD7" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BE7" s="4" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="BF7" s="4" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="BG7" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BH7" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="BI7" s="4" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="BJ7" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="BL7" s="6" t="s">
         <v>157</v>
@@ -4756,19 +4753,19 @@
         <v>156</v>
       </c>
       <c r="BN7" s="4" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="BO7" s="4" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="BP7" s="6" t="s">
         <v>158</v>
       </c>
       <c r="BQ7" s="4" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="BS7" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="BT7" s="11" t="b">
         <v>0</v>
@@ -4825,13 +4822,13 @@
         <v>101</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>102</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>103</v>
@@ -4932,7 +4929,7 @@
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
@@ -5001,7 +4998,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -5015,13 +5012,13 @@
         <v>130</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Added Step definition and test steps in Optimus Test case 2_1_2
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="342">
   <si>
     <t>Username</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>QA_TEST_2</t>
-  </si>
-  <si>
     <t>QA_TEST_3</t>
   </si>
   <si>
@@ -528,9 +525,6 @@
     <t>EIDTest1</t>
   </si>
   <si>
-    <t>EIDTest2</t>
-  </si>
-  <si>
     <t>EIDTest3</t>
   </si>
   <si>
@@ -603,9 +597,6 @@
     <t>Automation Test 1</t>
   </si>
   <si>
-    <t>Automation Test 2</t>
-  </si>
-  <si>
     <t>Automation Test 3</t>
   </si>
   <si>
@@ -666,9 +657,6 @@
     <t>TX Automate 1</t>
   </si>
   <si>
-    <t>TX Automate 2</t>
-  </si>
-  <si>
     <t>TX Automate 3</t>
   </si>
   <si>
@@ -684,9 +672,6 @@
     <t>IDNum1</t>
   </si>
   <si>
-    <t>IDNum2</t>
-  </si>
-  <si>
     <t>IDNum3</t>
   </si>
   <si>
@@ -735,9 +720,6 @@
     <t>TXA Appointment Others 1</t>
   </si>
   <si>
-    <t>TXA Appointment Others 2</t>
-  </si>
-  <si>
     <t>TXA Authorized Person 3</t>
   </si>
   <si>
@@ -771,9 +753,6 @@
     <t>TXA Group Association 1</t>
   </si>
   <si>
-    <t>TXA Group Association 2</t>
-  </si>
-  <si>
     <t>TXA Group Association 3</t>
   </si>
   <si>
@@ -786,9 +765,6 @@
     <t>TXA Client Tier remarks 1</t>
   </si>
   <si>
-    <t>TXA Client Tier remarks 2</t>
-  </si>
-  <si>
     <t>TXA Client Tier remarks 3</t>
   </si>
   <si>
@@ -813,9 +789,6 @@
     <t>TXA Execution Fee Rate 1</t>
   </si>
   <si>
-    <t>TXA Execution Fee Rate 2</t>
-  </si>
-  <si>
     <t>TXA Execution Fee Rate 3</t>
   </si>
   <si>
@@ -867,9 +840,6 @@
     <t>TXA Counterparty Remarks 1</t>
   </si>
   <si>
-    <t>TXA Counterparty Remarks 2</t>
-  </si>
-  <si>
     <t>TXA Counterparty Remarks 3</t>
   </si>
   <si>
@@ -888,9 +858,6 @@
     <t>2022-12-01 00:00:00</t>
   </si>
   <si>
-    <t>2022-12-01 00:00:01</t>
-  </si>
-  <si>
     <t>2022-12-01 00:00:02</t>
   </si>
   <si>
@@ -903,9 +870,6 @@
     <t>Txa Op Adr 1</t>
   </si>
   <si>
-    <t>Txa Op Adr 2</t>
-  </si>
-  <si>
     <t>Txa Op Adr 3</t>
   </si>
   <si>
@@ -945,9 +909,6 @@
     <t>TXA Ref Ext Rebate 1</t>
   </si>
   <si>
-    <t>TXA Ref Ext Rebate 2</t>
-  </si>
-  <si>
     <t>TXA Ref Ext Rebate 3</t>
   </si>
   <si>
@@ -990,64 +951,97 @@
     <t>ActionsTempField</t>
   </si>
   <si>
-    <t>SFIDTestUPDT2</t>
-  </si>
-  <si>
-    <t>NickNameExtTest UPDT 2</t>
-  </si>
-  <si>
-    <t>NNIntTXAUPDT3</t>
-  </si>
-  <si>
-    <t>Test Update 2</t>
-  </si>
-  <si>
-    <t>Automate Update 2</t>
-  </si>
-  <si>
-    <t>UPDT2Test2</t>
-  </si>
-  <si>
-    <t>UPDT3Test2</t>
-  </si>
-  <si>
-    <t>PEP Declaration Screening Remarks Automate Test 2 Update</t>
-  </si>
-  <si>
-    <t>RegisteredAddress Automate 2 Update</t>
-  </si>
-  <si>
-    <t>TXA Primary Business Activity Remarks 2 Update</t>
-  </si>
-  <si>
-    <t>TXA Source of Funds Remarks 2 Update</t>
-  </si>
-  <si>
     <t>0998877665511</t>
   </si>
   <si>
-    <t>abcUpdate@abc.com</t>
-  </si>
-  <si>
-    <t>TXA Authorized P 2 Update</t>
-  </si>
-  <si>
-    <t>TXA Business Purpose for R Update 2</t>
-  </si>
-  <si>
-    <t>TXA Risk Score Remarks 2 Update</t>
-  </si>
-  <si>
-    <t>TXA FacetoFace Verification Remarks 2 Update</t>
-  </si>
-  <si>
-    <t>TXA Vouched Remarks 2 Update</t>
-  </si>
-  <si>
-    <t>TXA Management Remarks 2 Update</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>SFIDTest</t>
+  </si>
+  <si>
+    <t>UPDT2</t>
+  </si>
+  <si>
+    <t>Update2</t>
+  </si>
+  <si>
+    <t>Update 2</t>
+  </si>
+  <si>
+    <t>2000-01-02</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Fund Management</t>
+  </si>
+  <si>
+    <t>2002-08-02 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-12-02 00:00:01</t>
+  </si>
+  <si>
+    <t>99887766554411</t>
+  </si>
+  <si>
+    <t>UPDT3</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Trust</t>
+  </si>
+  <si>
+    <t>Upd</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Walk-in</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>abc@abc.comup</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>2022-08-02 00:00:00</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Up2</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Updt</t>
+  </si>
+  <si>
+    <t>Update values only</t>
   </si>
 </sst>
 </file>
@@ -1244,25 +1238,6 @@
   </cellStyles>
   <dxfs count="73">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -2845,6 +2820,25 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2904,78 +2898,78 @@
   <autoFilter ref="A1:BU7"/>
   <tableColumns count="73">
     <tableColumn id="1" name="TestCaseID" dataDxfId="71"/>
-    <tableColumn id="73" name="ActionsTempField" dataDxfId="0"/>
-    <tableColumn id="2" name="CounterparyRef" dataDxfId="70"/>
-    <tableColumn id="3" name="NitroClientID" dataDxfId="69"/>
-    <tableColumn id="4" name="SalesForceID" dataDxfId="68"/>
-    <tableColumn id="5" name="ElwoodID" dataDxfId="67"/>
-    <tableColumn id="6" name="NicknameExternal" dataDxfId="66"/>
-    <tableColumn id="7" name="NicknameInternal" dataDxfId="65"/>
-    <tableColumn id="8" name="ParentAccount" dataDxfId="64"/>
-    <tableColumn id="9" name="FirstName" dataDxfId="63"/>
-    <tableColumn id="10" name="LastName" dataDxfId="62"/>
-    <tableColumn id="11" name="Gender" dataDxfId="61"/>
-    <tableColumn id="12" name="Nationality" dataDxfId="60"/>
-    <tableColumn id="13" name="DateofBirth" dataDxfId="59"/>
-    <tableColumn id="14" name="Occupation" dataDxfId="58"/>
-    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="57"/>
-    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="56"/>
-    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="55"/>
-    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="54"/>
-    <tableColumn id="19" name="MobileNumber" dataDxfId="53"/>
-    <tableColumn id="20" name="PEPDeclaration" dataDxfId="52"/>
-    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="51"/>
-    <tableColumn id="22" name="Alias" dataDxfId="50"/>
-    <tableColumn id="23" name="TIN1" dataDxfId="49"/>
-    <tableColumn id="24" name="TIN2" dataDxfId="48"/>
-    <tableColumn id="25" name="TIN3" dataDxfId="47"/>
-    <tableColumn id="26" name="CompanyName" dataDxfId="46"/>
-    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="45"/>
-    <tableColumn id="28" name="ClientType" dataDxfId="44"/>
-    <tableColumn id="29" name="EntityType" dataDxfId="43"/>
-    <tableColumn id="30" name="IdentificationNumber" dataDxfId="42"/>
-    <tableColumn id="31" name="IdentificationType" dataDxfId="41"/>
-    <tableColumn id="32" name="RegisteredAddress" dataDxfId="40"/>
-    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="39"/>
-    <tableColumn id="34" name="StateofIncorporation" dataDxfId="38"/>
-    <tableColumn id="35" name="OperatingAddress" dataDxfId="37"/>
-    <tableColumn id="36" name="CountryofOperation" dataDxfId="36"/>
-    <tableColumn id="37" name="OnboardingMode" dataDxfId="35"/>
-    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="34"/>
-    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="33"/>
+    <tableColumn id="73" name="ActionsTempField" dataDxfId="70"/>
+    <tableColumn id="2" name="CounterparyRef" dataDxfId="69"/>
+    <tableColumn id="3" name="NitroClientID" dataDxfId="68"/>
+    <tableColumn id="4" name="SalesForceID" dataDxfId="67"/>
+    <tableColumn id="5" name="ElwoodID" dataDxfId="66"/>
+    <tableColumn id="6" name="NicknameExternal" dataDxfId="65"/>
+    <tableColumn id="7" name="NicknameInternal" dataDxfId="64"/>
+    <tableColumn id="8" name="ParentAccount" dataDxfId="63"/>
+    <tableColumn id="9" name="FirstName" dataDxfId="62"/>
+    <tableColumn id="10" name="LastName" dataDxfId="61"/>
+    <tableColumn id="11" name="Gender" dataDxfId="60"/>
+    <tableColumn id="12" name="Nationality" dataDxfId="59"/>
+    <tableColumn id="13" name="DateofBirth" dataDxfId="58"/>
+    <tableColumn id="14" name="Occupation" dataDxfId="57"/>
+    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="56"/>
+    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="55"/>
+    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="54"/>
+    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="53"/>
+    <tableColumn id="19" name="MobileNumber" dataDxfId="52"/>
+    <tableColumn id="20" name="PEPDeclaration" dataDxfId="51"/>
+    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="50"/>
+    <tableColumn id="22" name="Alias" dataDxfId="49"/>
+    <tableColumn id="23" name="TIN1" dataDxfId="48"/>
+    <tableColumn id="24" name="TIN2" dataDxfId="47"/>
+    <tableColumn id="25" name="TIN3" dataDxfId="46"/>
+    <tableColumn id="26" name="CompanyName" dataDxfId="45"/>
+    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="44"/>
+    <tableColumn id="28" name="ClientType" dataDxfId="43"/>
+    <tableColumn id="29" name="EntityType" dataDxfId="42"/>
+    <tableColumn id="30" name="IdentificationNumber" dataDxfId="41"/>
+    <tableColumn id="31" name="IdentificationType" dataDxfId="40"/>
+    <tableColumn id="32" name="RegisteredAddress" dataDxfId="39"/>
+    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="38"/>
+    <tableColumn id="34" name="StateofIncorporation" dataDxfId="37"/>
+    <tableColumn id="35" name="OperatingAddress" dataDxfId="36"/>
+    <tableColumn id="36" name="CountryofOperation" dataDxfId="35"/>
+    <tableColumn id="37" name="OnboardingMode" dataDxfId="34"/>
+    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="33"/>
+    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
     <tableColumn id="40" name="CorporateWebsite"/>
-    <tableColumn id="41" name="GSTRegistered" dataDxfId="32"/>
-    <tableColumn id="42" name="FinancialInstitution" dataDxfId="31"/>
-    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="30"/>
-    <tableColumn id="44" name="SourceofFunds" dataDxfId="29"/>
-    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="28"/>
-    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="27"/>
-    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="26"/>
-    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="25"/>
-    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="24"/>
-    <tableColumn id="50" name="AppointmentOthers" dataDxfId="23"/>
-    <tableColumn id="51" name="GroupAssociation" dataDxfId="22"/>
-    <tableColumn id="52" name="OnboardedDate" dataDxfId="21"/>
-    <tableColumn id="53" name="ClientTier" dataDxfId="20"/>
-    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="19"/>
-    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="18"/>
-    <tableColumn id="56" name="RiskScore" dataDxfId="17"/>
-    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="16"/>
-    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="15"/>
-    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="14"/>
-    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="13"/>
-    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="12"/>
-    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="11"/>
-    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="10"/>
-    <tableColumn id="64" name="VouchedStatus" dataDxfId="9"/>
-    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="8"/>
-    <tableColumn id="66" name="VouchedRemarks" dataDxfId="7"/>
-    <tableColumn id="67" name="ManagementRemarks" dataDxfId="6"/>
-    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="5"/>
-    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="4"/>
-    <tableColumn id="70" name="Messages" dataDxfId="3"/>
-    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="2"/>
-    <tableColumn id="72" name="SIT" dataDxfId="1"/>
+    <tableColumn id="41" name="GSTRegistered" dataDxfId="31"/>
+    <tableColumn id="42" name="FinancialInstitution" dataDxfId="30"/>
+    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="29"/>
+    <tableColumn id="44" name="SourceofFunds" dataDxfId="28"/>
+    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="27"/>
+    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="26"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="25"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="24"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="23"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="22"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="21"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="20"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="19"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="18"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="17"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="16"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="15"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="14"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="13"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="12"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="11"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="8"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="7"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="6"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="5"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="4"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="3"/>
+    <tableColumn id="70" name="Messages" dataDxfId="2"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="72" name="SIT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3407,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BN4" sqref="BN4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3492,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>76</v>
@@ -3552,7 +3546,7 @@
         <v>33</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>19</v>
@@ -3639,7 +3633,7 @@
         <v>58</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="AZ1" s="4" t="s">
         <v>59</v>
@@ -3718,7 +3712,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -3726,17 +3720,17 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
@@ -3746,81 +3740,81 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
       <c r="AL2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AS2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ2" s="4"/>
       <c r="BA2" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="BB2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
       <c r="BE2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF2" s="4"/>
       <c r="BG2" s="4"/>
       <c r="BH2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BI2" s="5"/>
       <c r="BK2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BL2" s="4"/>
       <c r="BM2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BN2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BO2" s="4"/>
       <c r="BP2" s="4"/>
       <c r="BQ2" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BR2" s="4"/>
       <c r="BS2" s="13"/>
       <c r="BT2" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU2" s="11" t="b">
         <v>0</v>
@@ -3831,76 +3825,76 @@
         <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>144</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L3" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>189</v>
-      </c>
       <c r="N3" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>145</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>146</v>
       </c>
       <c r="R3" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>85</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AC3" s="4" t="s">
         <v>89</v>
@@ -3909,7 +3903,7 @@
         <v>90</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AF3" s="6" t="s">
         <v>147</v>
@@ -3924,7 +3918,7 @@
         <v>149</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="AK3" s="6" t="s">
         <v>148</v>
@@ -3936,70 +3930,70 @@
         <v>146</v>
       </c>
       <c r="AN3" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AO3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AS3" s="6" t="s">
         <v>151</v>
       </c>
       <c r="AT3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AX3" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="AU3" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="AV3" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>306</v>
-      </c>
-      <c r="AX3" s="4" t="s">
-        <v>237</v>
-      </c>
       <c r="AY3" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="AZ3" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="BA3" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BB3" s="6" t="s">
         <v>152</v>
       </c>
       <c r="BC3" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BD3" s="6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="BE3" s="6" t="s">
         <v>153</v>
       </c>
       <c r="BF3" s="4" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="BG3" s="4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="BH3" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BI3" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="BJ3" s="4" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="BK3" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BL3" s="4" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="BM3" s="6" t="s">
         <v>155</v>
@@ -4008,219 +4002,219 @@
         <v>154</v>
       </c>
       <c r="BO3" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="BP3" s="4" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="BQ3" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BR3" s="4" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="BT3" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU3" s="11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:73" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:73" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="V4" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AC4" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="AD4" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="AE4" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="J4" s="14" t="s">
+      <c r="AF4" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="AG4" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="AH4" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="V4" s="6" t="s">
+      <c r="AI4" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>332</v>
+      </c>
+      <c r="AS4" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="X4" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH4" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI4" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ4" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="AK4" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL4" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN4" s="6" t="s">
+      <c r="AT4" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="AV4" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="AW4" t="s">
         <v>333</v>
       </c>
-      <c r="AO4" t="s">
-        <v>231</v>
-      </c>
-      <c r="AS4" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT4" s="4" t="s">
+      <c r="AX4" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="AY4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="AU4" s="4" t="s">
+      <c r="BA4" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="BB4" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="BC4" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="BD4" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="BE4" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AV4" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>336</v>
-      </c>
-      <c r="AX4" s="4" t="s">
+      <c r="BF4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="BG4" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="BA4" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="BB4" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BC4" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="BD4" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BE4" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="BG4" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="BH4" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BI4" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="BJ4" s="4" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="BK4" s="6" t="s">
-        <v>343</v>
+        <v>312</v>
       </c>
       <c r="BL4" s="4" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="BM4" s="6" t="s">
-        <v>343</v>
+        <v>312</v>
       </c>
       <c r="BN4" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BO4" s="4" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="BP4" s="4" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="BQ4" s="6" t="s">
-        <v>156</v>
+        <v>339</v>
       </c>
       <c r="BR4" s="4" t="s">
-        <v>283</v>
+        <v>340</v>
       </c>
       <c r="BT4" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU4" s="11" t="b">
         <v>0</v>
@@ -4232,73 +4226,73 @@
       </c>
       <c r="B5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M5" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>145</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>146</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="T5" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="X5" s="6" t="s">
         <v>86</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AA5" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="AB5" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AC5" s="4" t="s">
         <v>89</v>
@@ -4307,7 +4301,7 @@
         <v>90</v>
       </c>
       <c r="AE5" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="AF5" s="6" t="s">
         <v>147</v>
@@ -4322,7 +4316,7 @@
         <v>149</v>
       </c>
       <c r="AJ5" s="6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="AK5" s="6" t="s">
         <v>148</v>
@@ -4334,70 +4328,70 @@
         <v>146</v>
       </c>
       <c r="AN5" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AO5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AS5" s="6" t="s">
         <v>151</v>
       </c>
       <c r="AT5" s="4" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AU5" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="AV5" s="4" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AW5" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AZ5" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="BA5" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BB5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="BC5" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BD5" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="BE5" s="6" t="s">
         <v>153</v>
       </c>
       <c r="BF5" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="BG5" s="4" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="BH5" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BI5" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="BJ5" s="4" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="BK5" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BL5" s="4" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="BM5" s="6" t="s">
         <v>155</v>
@@ -4406,19 +4400,19 @@
         <v>154</v>
       </c>
       <c r="BO5" s="4" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="BP5" s="4" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="BQ5" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BR5" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="BT5" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU5" s="11" t="b">
         <v>0</v>
@@ -4430,73 +4424,73 @@
       </c>
       <c r="B6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>145</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>146</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>87</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>89</v>
@@ -4505,7 +4499,7 @@
         <v>90</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AF6" s="6" t="s">
         <v>147</v>
@@ -4520,7 +4514,7 @@
         <v>149</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="AK6" s="6" t="s">
         <v>148</v>
@@ -4532,70 +4526,70 @@
         <v>146</v>
       </c>
       <c r="AN6" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AO6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AS6" s="6" t="s">
         <v>151</v>
       </c>
       <c r="AT6" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AV6" s="4" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AW6" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="AX6" s="4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AY6" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AZ6" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="BA6" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BB6" s="6" t="s">
         <v>152</v>
       </c>
       <c r="BC6" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BD6" s="6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="BE6" s="6" t="s">
         <v>153</v>
       </c>
       <c r="BF6" s="4" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="BG6" s="4" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="BH6" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BI6" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="BJ6" s="4" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="BK6" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BL6" s="4" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="BM6" s="6" t="s">
         <v>155</v>
@@ -4604,19 +4598,19 @@
         <v>154</v>
       </c>
       <c r="BO6" s="4" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="BQ6" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BR6" s="4" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="BT6" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU6" s="11" t="b">
         <v>0</v>
@@ -4628,73 +4622,73 @@
       </c>
       <c r="B7" s="5"/>
       <c r="D7" s="6" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>145</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>146</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>88</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="AB7" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AC7" s="4" t="s">
         <v>89</v>
@@ -4703,7 +4697,7 @@
         <v>90</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AF7" s="6" t="s">
         <v>147</v>
@@ -4718,7 +4712,7 @@
         <v>149</v>
       </c>
       <c r="AJ7" s="6" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="AK7" s="6" t="s">
         <v>148</v>
@@ -4730,70 +4724,70 @@
         <v>146</v>
       </c>
       <c r="AN7" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AO7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AS7" s="6" t="s">
         <v>151</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="AU7" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="AV7" s="4" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AW7" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="AX7" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="AY7" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="AZ7" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="AY7" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="AZ7" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="BA7" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BB7" s="6" t="s">
         <v>152</v>
       </c>
       <c r="BC7" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BD7" s="6" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="BE7" s="6" t="s">
         <v>153</v>
       </c>
       <c r="BF7" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="BG7" s="4" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="BH7" s="6" t="s">
         <v>154</v>
       </c>
       <c r="BI7" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="BJ7" s="4" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="BK7" s="6" t="s">
         <v>155</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="BM7" s="6" t="s">
         <v>155</v>
@@ -4802,19 +4796,19 @@
         <v>154</v>
       </c>
       <c r="BO7" s="4" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="BP7" s="4" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="BQ7" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BR7" s="4" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="BT7" s="11" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="BU7" s="11" t="b">
         <v>0</v>
@@ -4871,13 +4865,13 @@
         <v>99</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>100</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>101</v>
@@ -4978,7 +4972,7 @@
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
@@ -4997,13 +4991,13 @@
         <v>133</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P2" s="15" t="s">
         <v>134</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R2" s="15">
         <v>121212</v>
@@ -5013,10 +5007,10 @@
       </c>
       <c r="T2" s="15"/>
       <c r="U2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="V2" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
@@ -5047,7 +5041,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -5061,13 +5055,13 @@
         <v>128</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>129</v>
@@ -5085,13 +5079,13 @@
         <v>133</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>134</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R3" s="15">
         <v>121212</v>
@@ -5101,10 +5095,10 @@
       </c>
       <c r="T3" s="15"/>
       <c r="U3" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="V3" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>

</xml_diff>

<commit_message>
Delete CP TC QA_TestCase_Auto_Optimus_2_1_3
Updated excel, Feature file, Steps, Actions and locators
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
+    <workbookView minimized="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="311">
   <si>
     <t>Username</t>
   </si>
@@ -276,9 +276,6 @@
     <t>TIN1Test1</t>
   </si>
   <si>
-    <t>TIN1Test3</t>
-  </si>
-  <si>
     <t>TIN1Test4</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>RegisteredAddress Automate 1</t>
   </si>
   <si>
-    <t>RegisteredAddress Automate 3</t>
-  </si>
-  <si>
     <t>RegisteredAddress Automate 4</t>
   </si>
   <si>
@@ -489,9 +483,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>QA_TEST_3</t>
-  </si>
-  <si>
     <t>QA_TEST_4</t>
   </si>
   <si>
@@ -513,9 +504,6 @@
     <t>SFIDTest1</t>
   </si>
   <si>
-    <t>SFIDTest3</t>
-  </si>
-  <si>
     <t>SFIDTest4</t>
   </si>
   <si>
@@ -525,9 +513,6 @@
     <t>EIDTest1</t>
   </si>
   <si>
-    <t>EIDTest3</t>
-  </si>
-  <si>
     <t>EIDTest4</t>
   </si>
   <si>
@@ -537,9 +522,6 @@
     <t>NickNameExt Test 1</t>
   </si>
   <si>
-    <t>NickNameExt Test 3</t>
-  </si>
-  <si>
     <t>NickNameExt Test 4</t>
   </si>
   <si>
@@ -552,9 +534,6 @@
     <t>Test 1</t>
   </si>
   <si>
-    <t>Test 3</t>
-  </si>
-  <si>
     <t>Test 4</t>
   </si>
   <si>
@@ -564,9 +543,6 @@
     <t>Automate 1</t>
   </si>
   <si>
-    <t>Automate 3</t>
-  </si>
-  <si>
     <t>Automate 4</t>
   </si>
   <si>
@@ -585,9 +561,6 @@
     <t>Indian</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>UAE</t>
   </si>
   <si>
@@ -597,9 +570,6 @@
     <t>Automation Test 1</t>
   </si>
   <si>
-    <t>Automation Test 3</t>
-  </si>
-  <si>
     <t>Automation Test 4</t>
   </si>
   <si>
@@ -621,9 +591,6 @@
     <t>PEP Declaration Screening Remarks Automate Test 1</t>
   </si>
   <si>
-    <t>PEP Declaration Screening Remarks Automate Test 3</t>
-  </si>
-  <si>
     <t>PEP Declaration Screening Remarks Automate Test 4</t>
   </si>
   <si>
@@ -636,12 +603,6 @@
     <t>Tin3Test1</t>
   </si>
   <si>
-    <t>Tin2Test3</t>
-  </si>
-  <si>
-    <t>Tin3Test3</t>
-  </si>
-  <si>
     <t>Tin2Test4</t>
   </si>
   <si>
@@ -657,9 +618,6 @@
     <t>TX Automate 1</t>
   </si>
   <si>
-    <t>TX Automate 3</t>
-  </si>
-  <si>
     <t>TX Automate 4</t>
   </si>
   <si>
@@ -672,9 +630,6 @@
     <t>IDNum1</t>
   </si>
   <si>
-    <t>IDNum3</t>
-  </si>
-  <si>
     <t>IDNum4</t>
   </si>
   <si>
@@ -684,9 +639,6 @@
     <t>TXA Primary Business Activity Remarks 1</t>
   </si>
   <si>
-    <t>TXA Primary Business Activity Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Primary Business Activity Remarks 4</t>
   </si>
   <si>
@@ -702,9 +654,6 @@
     <t>TXA Source of Funds Remarks 1</t>
   </si>
   <si>
-    <t>TXA Source of Funds Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Source of Funds Remarks 4</t>
   </si>
   <si>
@@ -720,15 +669,6 @@
     <t>TXA Appointment Others 1</t>
   </si>
   <si>
-    <t>TXA Authorized Person 3</t>
-  </si>
-  <si>
-    <t>TXA Business Purpose for Relationship 3</t>
-  </si>
-  <si>
-    <t>TXA Appointment Others 3</t>
-  </si>
-  <si>
     <t>TXA Authorized Person 4</t>
   </si>
   <si>
@@ -753,9 +693,6 @@
     <t>TXA Group Association 1</t>
   </si>
   <si>
-    <t>TXA Group Association 3</t>
-  </si>
-  <si>
     <t>TXA Group Association 4</t>
   </si>
   <si>
@@ -765,9 +702,6 @@
     <t>TXA Client Tier remarks 1</t>
   </si>
   <si>
-    <t>TXA Client Tier remarks 3</t>
-  </si>
-  <si>
     <t>TXA Client Tier remarks 4</t>
   </si>
   <si>
@@ -777,9 +711,6 @@
     <t>TXA Risk Score Remarks 1</t>
   </si>
   <si>
-    <t>TXA Risk Score Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Risk Score Remarks 4</t>
   </si>
   <si>
@@ -789,9 +720,6 @@
     <t>TXA Execution Fee Rate 1</t>
   </si>
   <si>
-    <t>TXA Execution Fee Rate 3</t>
-  </si>
-  <si>
     <t>TXA Execution Fee Rate 4</t>
   </si>
   <si>
@@ -804,9 +732,6 @@
     <t>TXA FacetoFace Verification Remarks 1</t>
   </si>
   <si>
-    <t>TXA FacetoFace Verification Remarks 3</t>
-  </si>
-  <si>
     <t>TXA FacetoFace Verification Remarks 4</t>
   </si>
   <si>
@@ -816,9 +741,6 @@
     <t>TXA Vouched Remarks 1</t>
   </si>
   <si>
-    <t>TXA Vouched Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Vouched Remarks 4</t>
   </si>
   <si>
@@ -828,9 +750,6 @@
     <t>TXA Management Remarks 1</t>
   </si>
   <si>
-    <t>TXA Management Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Management Remarks 5</t>
   </si>
   <si>
@@ -840,9 +759,6 @@
     <t>TXA Counterparty Remarks 1</t>
   </si>
   <si>
-    <t>TXA Counterparty Remarks 3</t>
-  </si>
-  <si>
     <t>TXA Counterparty Remarks 4</t>
   </si>
   <si>
@@ -858,9 +774,6 @@
     <t>2022-12-01 00:00:00</t>
   </si>
   <si>
-    <t>2022-12-01 00:00:02</t>
-  </si>
-  <si>
     <t>2022-12-01 00:00:03</t>
   </si>
   <si>
@@ -870,9 +783,6 @@
     <t>Txa Op Adr 1</t>
   </si>
   <si>
-    <t>Txa Op Adr 3</t>
-  </si>
-  <si>
     <t>Txa Op Adr 4</t>
   </si>
   <si>
@@ -909,9 +819,6 @@
     <t>TXA Ref Ext Rebate 1</t>
   </si>
   <si>
-    <t>TXA Ref Ext Rebate 3</t>
-  </si>
-  <si>
     <t>TXA Ref Ext Rebate 4</t>
   </si>
   <si>
@@ -933,9 +840,6 @@
     <t>NNameIntTXA2</t>
   </si>
   <si>
-    <t>NNameIntTXA4</t>
-  </si>
-  <si>
     <t>NNameIntTXA5</t>
   </si>
   <si>
@@ -1042,6 +946,9 @@
   </si>
   <si>
     <t>Update values only</t>
+  </si>
+  <si>
+    <t>Delete</t>
   </si>
 </sst>
 </file>
@@ -3402,7 +3309,7 @@
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3410,8 +3317,8 @@
     <col min="1" max="1" width="31.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.54296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" style="6" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" style="6" customWidth="1"/>
     <col min="8" max="8" width="17.453125" style="6" bestFit="1" customWidth="1"/>
@@ -3486,7 +3393,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>76</v>
@@ -3534,7 +3441,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>31</v>
@@ -3546,7 +3453,7 @@
         <v>33</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>19</v>
@@ -3582,10 +3489,10 @@
         <v>43</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AJ1" s="4" t="s">
         <v>44</v>
@@ -3633,7 +3540,7 @@
         <v>58</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="AZ1" s="4" t="s">
         <v>59</v>
@@ -3660,10 +3567,10 @@
         <v>66</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BI1" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BJ1" s="4" t="s">
         <v>67</v>
@@ -3693,7 +3600,7 @@
         <v>75</v>
       </c>
       <c r="BS1" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="BT1" s="11" t="s">
         <v>11</v>
@@ -3712,7 +3619,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -3720,17 +3627,17 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
@@ -3740,81 +3647,81 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
       <c r="AL2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AM2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="AS2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AZ2" s="4"/>
       <c r="BA2" s="5" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="BB2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
       <c r="BE2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BF2" s="4"/>
       <c r="BG2" s="4"/>
       <c r="BH2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BI2" s="5"/>
       <c r="BK2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BL2" s="4"/>
       <c r="BM2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BN2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BO2" s="4"/>
       <c r="BP2" s="4"/>
       <c r="BQ2" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="BR2" s="4"/>
       <c r="BS2" s="13"/>
       <c r="BT2" s="11" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="BU2" s="11" t="b">
         <v>0</v>
@@ -3825,196 +3732,196 @@
         <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="G3" s="14" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="M3" s="14" t="s">
+      <c r="R3" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>197</v>
-      </c>
       <c r="S3" s="6" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>85</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="AB3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AY3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="AC3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL3" s="6" t="s">
+      <c r="AZ3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BB3" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="AM3" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AS3" s="6" t="s">
+      <c r="BC3" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BD3" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="BE3" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="AT3" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="AV3" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX3" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="AY3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BG3" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="AZ3" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="BA3" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB3" s="6" t="s">
+      <c r="BH3" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="BC3" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="BE3" s="6" t="s">
+      <c r="BI3" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BK3" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="BF3" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="BG3" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="BH3" s="6" t="s">
+      <c r="BL3" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="BM3" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="BO3" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="BP3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="BQ3" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="BI3" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="BJ3" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="BK3" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL3" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BM3" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN3" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BO3" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="BP3" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="BQ3" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="BR3" s="4" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="BT3" s="11" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="BU3" s="11" t="b">
         <v>0</v>
@@ -4025,196 +3932,196 @@
         <v>81</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH4" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="AI4" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AO4" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="AH4" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="AI4" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="AJ4" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="AK4" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="AL4" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="AM4" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>332</v>
-      </c>
       <c r="AS4" s="6" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="AW4" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="AX4" s="4" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="AY4" s="4" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="AZ4" s="4" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="BA4" s="6" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="BB4" s="6" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="BC4" s="6" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="BD4" s="6" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="BE4" s="6" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="BF4" s="4" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="BG4" s="4" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="BH4" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BI4" s="6" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="BJ4" s="4" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="BK4" s="6" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="BL4" s="4" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="BM4" s="6" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="BN4" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BO4" s="4" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="BP4" s="4" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="BQ4" s="6" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="BR4" s="4" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="BT4" s="11" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="BU4" s="11" t="b">
         <v>0</v>
@@ -4224,195 +4131,43 @@
       <c r="A5" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>310</v>
+      </c>
       <c r="D5" s="6" t="s">
-        <v>301</v>
+        <v>270</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH5" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI5" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL5" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM5" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>225</v>
-      </c>
-      <c r="AS5" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="BA5" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB5" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BC5" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BD5" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="BE5" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="BH5" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BI5" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="BJ5" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="BK5" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL5" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="BM5" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN5" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BO5" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="BP5" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="BQ5" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="BR5" s="4" t="s">
-        <v>274</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="AC5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AO5"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5"/>
+      <c r="AX5" s="4"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
+      <c r="BF5" s="4"/>
+      <c r="BG5" s="4"/>
+      <c r="BJ5" s="4"/>
+      <c r="BL5" s="4"/>
+      <c r="BO5" s="4"/>
+      <c r="BP5" s="4"/>
+      <c r="BR5" s="4"/>
       <c r="BT5" s="11" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="BU5" s="11" t="b">
         <v>0</v>
@@ -4424,193 +4179,193 @@
       </c>
       <c r="B6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="L6" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH6" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI6" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT6" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AV6" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA6" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="M6" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI6" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL6" s="6" t="s">
+      <c r="BB6" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="AM6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>226</v>
-      </c>
-      <c r="AS6" s="6" t="s">
+      <c r="BC6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BD6" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="BE6" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="AT6" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AU6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="AV6" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX6" s="4" t="s">
+      <c r="BF6" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="BG6" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="BH6" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="BI6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="BJ6" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="BK6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BL6" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="AY6" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="BA6" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB6" s="6" t="s">
+      <c r="BM6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN6" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="BC6" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BD6" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="BE6" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF6" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="BG6" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="BH6" s="6" t="s">
+      <c r="BO6" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="BP6" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="BQ6" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="BI6" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="BJ6" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="BK6" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL6" s="4" t="s">
+      <c r="BR6" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="BT6" s="11" t="s">
         <v>263</v>
-      </c>
-      <c r="BM6" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN6" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BO6" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BP6" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="BQ6" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="BR6" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="BT6" s="11" t="s">
-        <v>293</v>
       </c>
       <c r="BU6" s="11" t="b">
         <v>0</v>
@@ -4622,193 +4377,193 @@
       </c>
       <c r="B7" s="5"/>
       <c r="D7" s="6" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J7" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="M7" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="L7" s="14" t="s">
+      <c r="N7" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="Q7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="T7" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O7" s="6" t="s">
+      <c r="V7" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF7" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q7" s="6" t="s">
+      <c r="AG7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH7" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE7" s="6" t="s">
+      <c r="AI7" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ7" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="AK7" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN7" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS7" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT7" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU7" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="AF7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH7" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI7" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AK7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL7" s="6" t="s">
+      <c r="AV7" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX7" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AY7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AZ7" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="BA7" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BB7" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="AM7" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN7" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AS7" s="6" t="s">
+      <c r="BC7" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BD7" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="BE7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="AT7" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AU7" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="AV7" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX7" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="AY7" s="4" t="s">
+      <c r="BF7" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="BG7" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="BH7" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="BI7" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="BJ7" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="BK7" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BL7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="BM7" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN7" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="BO7" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="AZ7" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="BA7" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB7" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BC7" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="BD7" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="BE7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BF7" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="BG7" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="BH7" s="6" t="s">
+      <c r="BP7" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="BQ7" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="BI7" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="BJ7" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="BK7" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL7" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="BM7" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN7" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BO7" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="BP7" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="BQ7" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="BR7" s="4" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="BT7" s="11" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="BU7" s="11" t="b">
         <v>0</v>
@@ -4850,103 +4605,103 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="I1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH1" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="AI1" s="15" t="s">
         <v>11</v>
@@ -4957,47 +4712,47 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="15">
         <v>2710</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="O2" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>134</v>
-      </c>
       <c r="Q2" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R2" s="15">
         <v>121212</v>
@@ -5007,10 +4762,10 @@
       </c>
       <c r="T2" s="15"/>
       <c r="U2" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="V2" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
@@ -5018,13 +4773,13 @@
         <v>1434444</v>
       </c>
       <c r="Z2" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB2" s="15" t="s">
         <v>135</v>
-      </c>
-      <c r="AA2" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="AC2" s="15"/>
       <c r="AD2" s="15"/>
@@ -5041,51 +4796,51 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="15">
         <v>2710</v>
       </c>
       <c r="F3" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="O3" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="N3" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>134</v>
-      </c>
       <c r="Q3" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R3" s="15">
         <v>121212</v>
@@ -5095,10 +4850,10 @@
       </c>
       <c r="T3" s="15"/>
       <c r="U3" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="V3" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
@@ -5106,13 +4861,13 @@
         <v>1434444</v>
       </c>
       <c r="Z3" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB3" s="15" t="s">
         <v>135</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="AC3" s="15"/>
       <c r="AD3" s="15"/>

</xml_diff>

<commit_message>
Added New  testcase QA_Optimus _3_1_3
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A5C705-1A20-450C-832E-233706119C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="314">
   <si>
     <t>Username</t>
   </si>
@@ -949,12 +950,21 @@
   </si>
   <si>
     <t>Delete</t>
+  </si>
+  <si>
+    <t>Delete Settlement textbox</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_3_1_3</t>
+  </si>
+  <si>
+    <t>Delete Settlement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2801,82 +2811,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="72">
-  <autoFilter ref="A1:BU7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="72">
+  <autoFilter ref="A1:BU7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="73">
-    <tableColumn id="1" name="TestCaseID" dataDxfId="71"/>
-    <tableColumn id="73" name="ActionsTempField" dataDxfId="70"/>
-    <tableColumn id="2" name="CounterparyRef" dataDxfId="69"/>
-    <tableColumn id="3" name="NitroClientID" dataDxfId="68"/>
-    <tableColumn id="4" name="SalesForceID" dataDxfId="67"/>
-    <tableColumn id="5" name="ElwoodID" dataDxfId="66"/>
-    <tableColumn id="6" name="NicknameExternal" dataDxfId="65"/>
-    <tableColumn id="7" name="NicknameInternal" dataDxfId="64"/>
-    <tableColumn id="8" name="ParentAccount" dataDxfId="63"/>
-    <tableColumn id="9" name="FirstName" dataDxfId="62"/>
-    <tableColumn id="10" name="LastName" dataDxfId="61"/>
-    <tableColumn id="11" name="Gender" dataDxfId="60"/>
-    <tableColumn id="12" name="Nationality" dataDxfId="59"/>
-    <tableColumn id="13" name="DateofBirth" dataDxfId="58"/>
-    <tableColumn id="14" name="Occupation" dataDxfId="57"/>
-    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="56"/>
-    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="55"/>
-    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="54"/>
-    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="53"/>
-    <tableColumn id="19" name="MobileNumber" dataDxfId="52"/>
-    <tableColumn id="20" name="PEPDeclaration" dataDxfId="51"/>
-    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="50"/>
-    <tableColumn id="22" name="Alias" dataDxfId="49"/>
-    <tableColumn id="23" name="TIN1" dataDxfId="48"/>
-    <tableColumn id="24" name="TIN2" dataDxfId="47"/>
-    <tableColumn id="25" name="TIN3" dataDxfId="46"/>
-    <tableColumn id="26" name="CompanyName" dataDxfId="45"/>
-    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="44"/>
-    <tableColumn id="28" name="ClientType" dataDxfId="43"/>
-    <tableColumn id="29" name="EntityType" dataDxfId="42"/>
-    <tableColumn id="30" name="IdentificationNumber" dataDxfId="41"/>
-    <tableColumn id="31" name="IdentificationType" dataDxfId="40"/>
-    <tableColumn id="32" name="RegisteredAddress" dataDxfId="39"/>
-    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="38"/>
-    <tableColumn id="34" name="StateofIncorporation" dataDxfId="37"/>
-    <tableColumn id="35" name="OperatingAddress" dataDxfId="36"/>
-    <tableColumn id="36" name="CountryofOperation" dataDxfId="35"/>
-    <tableColumn id="37" name="OnboardingMode" dataDxfId="34"/>
-    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="33"/>
-    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
-    <tableColumn id="40" name="CorporateWebsite"/>
-    <tableColumn id="41" name="GSTRegistered" dataDxfId="31"/>
-    <tableColumn id="42" name="FinancialInstitution" dataDxfId="30"/>
-    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="29"/>
-    <tableColumn id="44" name="SourceofFunds" dataDxfId="28"/>
-    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="27"/>
-    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="26"/>
-    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="25"/>
-    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="24"/>
-    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="23"/>
-    <tableColumn id="50" name="AppointmentOthers" dataDxfId="22"/>
-    <tableColumn id="51" name="GroupAssociation" dataDxfId="21"/>
-    <tableColumn id="52" name="OnboardedDate" dataDxfId="20"/>
-    <tableColumn id="53" name="ClientTier" dataDxfId="19"/>
-    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="18"/>
-    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="17"/>
-    <tableColumn id="56" name="RiskScore" dataDxfId="16"/>
-    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="15"/>
-    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="14"/>
-    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="13"/>
-    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="12"/>
-    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="11"/>
-    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
-    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
-    <tableColumn id="64" name="VouchedStatus" dataDxfId="8"/>
-    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="7"/>
-    <tableColumn id="66" name="VouchedRemarks" dataDxfId="6"/>
-    <tableColumn id="67" name="ManagementRemarks" dataDxfId="5"/>
-    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="4"/>
-    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="3"/>
-    <tableColumn id="70" name="Messages" dataDxfId="2"/>
-    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="1"/>
-    <tableColumn id="72" name="SIT" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TestCaseID" dataDxfId="71"/>
+    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="ActionsTempField" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CounterparyRef" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NitroClientID" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SalesForceID" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ElwoodID" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NicknameExternal" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NicknameInternal" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ParentAccount" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FirstName" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="LastName" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nationality" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DateofBirth" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Occupation" dataDxfId="57"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CompanyofEmployment" dataDxfId="56"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IndustryofEmployment" dataDxfId="55"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IdentificationIssueDate" dataDxfId="54"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IdentificationExpiryDate" dataDxfId="53"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MobileNumber" dataDxfId="52"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PEPDeclaration" dataDxfId="51"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="PEPDeclarationRemarks" dataDxfId="50"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Alias" dataDxfId="49"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TIN1" dataDxfId="48"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TIN2" dataDxfId="47"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="TIN3" dataDxfId="46"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CompanyName" dataDxfId="45"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="FormerRegisteredName" dataDxfId="44"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ClientType" dataDxfId="43"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="EntityType" dataDxfId="42"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IdentificationNumber" dataDxfId="41"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="IdentificationType" dataDxfId="40"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="RegisteredAddress" dataDxfId="39"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="CountryofIncorporation" dataDxfId="38"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="StateofIncorporation" dataDxfId="37"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="OperatingAddress" dataDxfId="36"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="CountryofOperation" dataDxfId="35"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="OnboardingMode" dataDxfId="34"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="PrimaryBusinessActivity" dataDxfId="33"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="CorporateWebsite"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="GSTRegistered" dataDxfId="31"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="FinancialInstitution" dataDxfId="30"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PaymentServiceProvider" dataDxfId="29"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="SourceofFunds" dataDxfId="28"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="SourceofFundsRemarks" dataDxfId="27"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="AuthorizedPerson" dataDxfId="26"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="AuthorizedPersonMobile" dataDxfId="25"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="AuthorizedPersonEmail" dataDxfId="24"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="BusinessPurposeforRelationship" dataDxfId="23"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="AppointmentOthers" dataDxfId="22"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="GroupAssociation" dataDxfId="21"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="OnboardedDate" dataDxfId="20"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="ClientTier" dataDxfId="19"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="KYCRefreshDate" dataDxfId="18"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="ClientTierRemarks" dataDxfId="17"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RiskScore" dataDxfId="16"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RiskScoreRemarks" dataDxfId="15"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="ExecutionFeeRate" dataDxfId="14"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="ReferralPersonInternal" dataDxfId="13"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="ReferralPersonExternal" dataDxfId="12"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="ReferralExternalRebate" dataDxfId="11"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="VouchedStatus" dataDxfId="8"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="VouchedbyPerson" dataDxfId="7"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="VouchedRemarks" dataDxfId="6"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="ManagementRemarks" dataDxfId="5"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="CounterpartyStatus" dataDxfId="4"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="CounterpartyRemarks" dataDxfId="3"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Messages" dataDxfId="2"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="SIT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2958,6 +2968,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2993,6 +3020,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3168,7 +3212,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3295,9 +3339,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -3305,11 +3349,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4579,11 +4623,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4600,7 +4644,7 @@
     <col min="14" max="14" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -4698,19 +4742,22 @@
         <v>121</v>
       </c>
       <c r="AG1" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AH1" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>124</v>
       </c>
@@ -4787,14 +4834,15 @@
       <c r="AF2" s="15"/>
       <c r="AG2" s="15"/>
       <c r="AH2" s="15"/>
-      <c r="AI2" s="15">
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15">
         <v>1</v>
       </c>
-      <c r="AJ2" s="15" t="b">
+      <c r="AK2" s="15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>260</v>
       </c>
@@ -4875,10 +4923,102 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="15"/>
-      <c r="AI3" s="15">
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15">
         <v>1</v>
       </c>
-      <c r="AJ3" s="15" t="b">
+      <c r="AK3" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="15">
+        <v>2710</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="R4" s="15">
+        <v>121212</v>
+      </c>
+      <c r="S4" s="15">
+        <v>121</v>
+      </c>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15">
+        <v>1434444</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA4" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB4" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QA_TestCase_Auto_Optimus_2_2_1 Page file and Feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A5C705-1A20-450C-832E-233706119C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
     <sheet name="CreateCounterParty" sheetId="11" r:id="rId2"/>
-    <sheet name="Settlement" sheetId="12" r:id="rId3"/>
+    <sheet name="RelatedCounterParty" sheetId="13" r:id="rId3"/>
+    <sheet name="Settlement" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="273">
   <si>
     <t>Username</t>
   </si>
@@ -277,12 +277,6 @@
     <t>TIN1Test1</t>
   </si>
   <si>
-    <t>TIN1Test4</t>
-  </si>
-  <si>
-    <t>TIN1Test5</t>
-  </si>
-  <si>
     <t>Individual</t>
   </si>
   <si>
@@ -292,12 +286,6 @@
     <t>RegisteredAddress Automate 1</t>
   </si>
   <si>
-    <t>RegisteredAddress Automate 4</t>
-  </si>
-  <si>
-    <t>RegisteredAddress Automate 5</t>
-  </si>
-  <si>
     <t>Settlement Ref.</t>
   </si>
   <si>
@@ -487,9 +475,6 @@
     <t>QA_TEST_4</t>
   </si>
   <si>
-    <t>QA_TEST_5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Self Custody </t>
   </si>
   <si>
@@ -505,51 +490,21 @@
     <t>SFIDTest1</t>
   </si>
   <si>
-    <t>SFIDTest4</t>
-  </si>
-  <si>
-    <t>SFIDTest5</t>
-  </si>
-  <si>
     <t>EIDTest1</t>
   </si>
   <si>
-    <t>EIDTest4</t>
-  </si>
-  <si>
-    <t>EIDTest5</t>
-  </si>
-  <si>
     <t>NickNameExt Test 1</t>
   </si>
   <si>
-    <t>NickNameExt Test 4</t>
-  </si>
-  <si>
-    <t>NickNameExt Test 5</t>
-  </si>
-  <si>
     <t>Dropdown</t>
   </si>
   <si>
     <t>Test 1</t>
   </si>
   <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
     <t>Automate 1</t>
   </si>
   <si>
-    <t>Automate 4</t>
-  </si>
-  <si>
-    <t>Automate 5</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -562,21 +517,12 @@
     <t>Indian</t>
   </si>
   <si>
-    <t>UAE</t>
-  </si>
-  <si>
     <t>2000-01-01</t>
   </si>
   <si>
     <t>Automation Test 1</t>
   </si>
   <si>
-    <t>Automation Test 4</t>
-  </si>
-  <si>
-    <t>Automation Test 5</t>
-  </si>
-  <si>
     <t>2022-08-01 00:00:00</t>
   </si>
   <si>
@@ -592,75 +538,30 @@
     <t>PEP Declaration Screening Remarks Automate Test 1</t>
   </si>
   <si>
-    <t>PEP Declaration Screening Remarks Automate Test 4</t>
-  </si>
-  <si>
-    <t>PEP Declaration Screening Remarks Automate Test 5</t>
-  </si>
-  <si>
     <t>Tin2Test1</t>
   </si>
   <si>
     <t>Tin3Test1</t>
   </si>
   <si>
-    <t>Tin2Test4</t>
-  </si>
-  <si>
-    <t>Tin3Test4</t>
-  </si>
-  <si>
-    <t>Tin2Test5</t>
-  </si>
-  <si>
-    <t>Tin3Test5</t>
-  </si>
-  <si>
     <t>TX Automate 1</t>
   </si>
   <si>
-    <t>TX Automate 4</t>
-  </si>
-  <si>
-    <t>TX Automate 5</t>
-  </si>
-  <si>
     <t>TXA F Registered Name</t>
   </si>
   <si>
     <t>IDNum1</t>
   </si>
   <si>
-    <t>IDNum4</t>
-  </si>
-  <si>
-    <t>IDNum5</t>
-  </si>
-  <si>
     <t>TXA Primary Business Activity Remarks 1</t>
   </si>
   <si>
-    <t>TXA Primary Business Activity Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Primary Business Activity Remarks 5</t>
-  </si>
-  <si>
     <t>www.CorporateWebsiteX.com</t>
   </si>
   <si>
-    <t>Https://www.CorporateWebsiteX.com</t>
-  </si>
-  <si>
     <t>TXA Source of Funds Remarks 1</t>
   </si>
   <si>
-    <t>TXA Source of Funds Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Source of Funds Remarks 5</t>
-  </si>
-  <si>
     <t>TXA Authorized Person 1</t>
   </si>
   <si>
@@ -670,102 +571,36 @@
     <t>TXA Appointment Others 1</t>
   </si>
   <si>
-    <t>TXA Authorized Person 4</t>
-  </si>
-  <si>
-    <t>TXA Business Purpose for Relationship 4</t>
-  </si>
-  <si>
-    <t>TXA Appointment Others 4</t>
-  </si>
-  <si>
-    <t>TXA Authorized Person 5</t>
-  </si>
-  <si>
-    <t>TXA Business Purpose for Relationship 5</t>
-  </si>
-  <si>
-    <t>TXA Appointment Others 5</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>TXA Group Association 1</t>
   </si>
   <si>
-    <t>TXA Group Association 4</t>
-  </si>
-  <si>
-    <t>TXA Group Association 5</t>
-  </si>
-  <si>
     <t>TXA Client Tier remarks 1</t>
   </si>
   <si>
-    <t>TXA Client Tier remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Client Tier remarks 5</t>
-  </si>
-  <si>
     <t>TXA Risk Score Remarks 1</t>
   </si>
   <si>
-    <t>TXA Risk Score Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Risk Score Remarks 5</t>
-  </si>
-  <si>
     <t>TXA Execution Fee Rate 1</t>
   </si>
   <si>
-    <t>TXA Execution Fee Rate 4</t>
-  </si>
-  <si>
-    <t>TXA Execution Fee Rate 5</t>
-  </si>
-  <si>
     <t>amit.verma - -97</t>
   </si>
   <si>
     <t>TXA FacetoFace Verification Remarks 1</t>
   </si>
   <si>
-    <t>TXA FacetoFace Verification Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA FacetoFace Verification Remarks 5</t>
-  </si>
-  <si>
     <t>TXA Vouched Remarks 1</t>
   </si>
   <si>
-    <t>TXA Vouched Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Vouched Remarks 5</t>
-  </si>
-  <si>
     <t>TXA Management Remarks 1</t>
   </si>
   <si>
-    <t>TXA Management Remarks 5</t>
-  </si>
-  <si>
-    <t>TXA Management Remarks 4</t>
-  </si>
-  <si>
     <t>TXA Counterparty Remarks 1</t>
   </si>
   <si>
-    <t>TXA Counterparty Remarks 4</t>
-  </si>
-  <si>
-    <t>TXA Counterparty Remarks 5</t>
-  </si>
-  <si>
     <t>PEPDeclarationRemarks</t>
   </si>
   <si>
@@ -775,21 +610,9 @@
     <t>2022-12-01 00:00:00</t>
   </si>
   <si>
-    <t>2022-12-01 00:00:03</t>
-  </si>
-  <si>
-    <t>2022-12-01 00:00:04</t>
-  </si>
-  <si>
     <t>Txa Op Adr 1</t>
   </si>
   <si>
-    <t>Txa Op Adr 4</t>
-  </si>
-  <si>
-    <t>Txa Op Adr 5</t>
-  </si>
-  <si>
     <t>Settlement Nickname External Updated</t>
   </si>
   <si>
@@ -820,12 +643,6 @@
     <t>TXA Ref Ext Rebate 1</t>
   </si>
   <si>
-    <t>TXA Ref Ext Rebate 4</t>
-  </si>
-  <si>
-    <t>TXA Ref Ext Rebate 5</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -841,12 +658,6 @@
     <t>NNameIntTXA2</t>
   </si>
   <si>
-    <t>NNameIntTXA5</t>
-  </si>
-  <si>
-    <t>NNameIntTXA6</t>
-  </si>
-  <si>
     <t>Create</t>
   </si>
   <si>
@@ -959,13 +770,79 @@
   </si>
   <si>
     <t>Delete Settlement</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Download CSV Btn</t>
+  </si>
+  <si>
+    <t>TXA</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_2_1</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>RelatedPartyRef.</t>
+  </si>
+  <si>
+    <t>Counterparty</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>SourceOfFunds</t>
+  </si>
+  <si>
+    <t>SourceOfFundsRemarks</t>
+  </si>
+  <si>
+    <t>PEP</t>
+  </si>
+  <si>
+    <t>UltimateShareholding</t>
+  </si>
+  <si>
+    <t>SourceOfWealth</t>
+  </si>
+  <si>
+    <t>SourceOfWealthRemarks</t>
+  </si>
+  <si>
+    <t>Appointment</t>
+  </si>
+  <si>
+    <t>AppointmentAppointDate</t>
+  </si>
+  <si>
+    <t>AppointmentResignDate</t>
+  </si>
+  <si>
+    <t>CountryOfIncorporation</t>
+  </si>
+  <si>
+    <t>StateOfIncorporation</t>
+  </si>
+  <si>
+    <t>OperationAddress</t>
+  </si>
+  <si>
+    <t>CountryOfOperation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -987,6 +864,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -996,7 +881,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1103,11 +988,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1149,6 +1047,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2811,82 +2719,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="72">
-  <autoFilter ref="A1:BU7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="72">
+  <autoFilter ref="A1:BU7"/>
   <tableColumns count="73">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TestCaseID" dataDxfId="71"/>
-    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="ActionsTempField" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CounterparyRef" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NitroClientID" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SalesForceID" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ElwoodID" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NicknameExternal" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NicknameInternal" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ParentAccount" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FirstName" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="LastName" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nationality" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DateofBirth" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Occupation" dataDxfId="57"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CompanyofEmployment" dataDxfId="56"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IndustryofEmployment" dataDxfId="55"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IdentificationIssueDate" dataDxfId="54"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IdentificationExpiryDate" dataDxfId="53"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MobileNumber" dataDxfId="52"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PEPDeclaration" dataDxfId="51"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="PEPDeclarationRemarks" dataDxfId="50"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Alias" dataDxfId="49"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TIN1" dataDxfId="48"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TIN2" dataDxfId="47"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="TIN3" dataDxfId="46"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CompanyName" dataDxfId="45"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="FormerRegisteredName" dataDxfId="44"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ClientType" dataDxfId="43"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="EntityType" dataDxfId="42"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IdentificationNumber" dataDxfId="41"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="IdentificationType" dataDxfId="40"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="RegisteredAddress" dataDxfId="39"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="CountryofIncorporation" dataDxfId="38"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="StateofIncorporation" dataDxfId="37"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="OperatingAddress" dataDxfId="36"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="CountryofOperation" dataDxfId="35"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="OnboardingMode" dataDxfId="34"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="PrimaryBusinessActivity" dataDxfId="33"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="CorporateWebsite"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="GSTRegistered" dataDxfId="31"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="FinancialInstitution" dataDxfId="30"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PaymentServiceProvider" dataDxfId="29"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="SourceofFunds" dataDxfId="28"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="SourceofFundsRemarks" dataDxfId="27"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="AuthorizedPerson" dataDxfId="26"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="AuthorizedPersonMobile" dataDxfId="25"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="AuthorizedPersonEmail" dataDxfId="24"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="BusinessPurposeforRelationship" dataDxfId="23"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="AppointmentOthers" dataDxfId="22"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="GroupAssociation" dataDxfId="21"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="OnboardedDate" dataDxfId="20"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="ClientTier" dataDxfId="19"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="KYCRefreshDate" dataDxfId="18"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="ClientTierRemarks" dataDxfId="17"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RiskScore" dataDxfId="16"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RiskScoreRemarks" dataDxfId="15"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="ExecutionFeeRate" dataDxfId="14"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="ReferralPersonInternal" dataDxfId="13"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="ReferralPersonExternal" dataDxfId="12"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="ReferralExternalRebate" dataDxfId="11"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="VouchedStatus" dataDxfId="8"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="VouchedbyPerson" dataDxfId="7"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="VouchedRemarks" dataDxfId="6"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="ManagementRemarks" dataDxfId="5"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="CounterpartyStatus" dataDxfId="4"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="CounterpartyRemarks" dataDxfId="3"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Messages" dataDxfId="2"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="SkipAtStepNum" dataDxfId="1"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="SIT" dataDxfId="0"/>
+    <tableColumn id="1" name="TestCaseID" dataDxfId="71"/>
+    <tableColumn id="73" name="ActionsTempField" dataDxfId="70"/>
+    <tableColumn id="2" name="CounterparyRef" dataDxfId="69"/>
+    <tableColumn id="3" name="NitroClientID" dataDxfId="68"/>
+    <tableColumn id="4" name="SalesForceID" dataDxfId="67"/>
+    <tableColumn id="5" name="ElwoodID" dataDxfId="66"/>
+    <tableColumn id="6" name="NicknameExternal" dataDxfId="65"/>
+    <tableColumn id="7" name="NicknameInternal" dataDxfId="64"/>
+    <tableColumn id="8" name="ParentAccount" dataDxfId="63"/>
+    <tableColumn id="9" name="FirstName" dataDxfId="62"/>
+    <tableColumn id="10" name="LastName" dataDxfId="61"/>
+    <tableColumn id="11" name="Gender" dataDxfId="60"/>
+    <tableColumn id="12" name="Nationality" dataDxfId="59"/>
+    <tableColumn id="13" name="DateofBirth" dataDxfId="58"/>
+    <tableColumn id="14" name="Occupation" dataDxfId="57"/>
+    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="56"/>
+    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="55"/>
+    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="54"/>
+    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="53"/>
+    <tableColumn id="19" name="MobileNumber" dataDxfId="52"/>
+    <tableColumn id="20" name="PEPDeclaration" dataDxfId="51"/>
+    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="50"/>
+    <tableColumn id="22" name="Alias" dataDxfId="49"/>
+    <tableColumn id="23" name="TIN1" dataDxfId="48"/>
+    <tableColumn id="24" name="TIN2" dataDxfId="47"/>
+    <tableColumn id="25" name="TIN3" dataDxfId="46"/>
+    <tableColumn id="26" name="CompanyName" dataDxfId="45"/>
+    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="44"/>
+    <tableColumn id="28" name="ClientType" dataDxfId="43"/>
+    <tableColumn id="29" name="EntityType" dataDxfId="42"/>
+    <tableColumn id="30" name="IdentificationNumber" dataDxfId="41"/>
+    <tableColumn id="31" name="IdentificationType" dataDxfId="40"/>
+    <tableColumn id="32" name="RegisteredAddress" dataDxfId="39"/>
+    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="38"/>
+    <tableColumn id="34" name="StateofIncorporation" dataDxfId="37"/>
+    <tableColumn id="35" name="OperatingAddress" dataDxfId="36"/>
+    <tableColumn id="36" name="CountryofOperation" dataDxfId="35"/>
+    <tableColumn id="37" name="OnboardingMode" dataDxfId="34"/>
+    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="33"/>
+    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
+    <tableColumn id="40" name="CorporateWebsite"/>
+    <tableColumn id="41" name="GSTRegistered" dataDxfId="31"/>
+    <tableColumn id="42" name="FinancialInstitution" dataDxfId="30"/>
+    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="29"/>
+    <tableColumn id="44" name="SourceofFunds" dataDxfId="28"/>
+    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="27"/>
+    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="26"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="25"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="24"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="23"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="22"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="21"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="20"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="19"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="18"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="17"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="16"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="15"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="14"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="13"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="12"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="11"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="8"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="7"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="6"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="5"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="4"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="3"/>
+    <tableColumn id="70" name="Messages" dataDxfId="2"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="72" name="SIT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2968,23 +2876,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3020,23 +2911,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3212,7 +3086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3339,9 +3213,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -3349,12 +3223,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3437,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>278</v>
+        <v>215</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>76</v>
@@ -3485,7 +3357,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>31</v>
@@ -3497,7 +3369,7 @@
         <v>33</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>249</v>
+        <v>194</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>19</v>
@@ -3533,10 +3405,10 @@
         <v>43</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AJ1" s="4" t="s">
         <v>44</v>
@@ -3584,7 +3456,7 @@
         <v>58</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>250</v>
+        <v>195</v>
       </c>
       <c r="AZ1" s="4" t="s">
         <v>59</v>
@@ -3611,10 +3483,10 @@
         <v>66</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="BI1" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="BJ1" s="4" t="s">
         <v>67</v>
@@ -3644,7 +3516,7 @@
         <v>75</v>
       </c>
       <c r="BS1" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="BT1" s="11" t="s">
         <v>11</v>
@@ -3663,7 +3535,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -3671,17 +3543,17 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
@@ -3691,81 +3563,81 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AG2" s="4"/>
       <c r="AH2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
       <c r="AL2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AM2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="AS2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="AZ2" s="4"/>
       <c r="BA2" s="5" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="BB2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
       <c r="BE2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BF2" s="4"/>
       <c r="BG2" s="4"/>
       <c r="BH2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BI2" s="5"/>
       <c r="BK2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BL2" s="4"/>
       <c r="BM2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BN2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BO2" s="4"/>
       <c r="BP2" s="4"/>
       <c r="BQ2" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="BR2" s="4"/>
       <c r="BS2" s="13"/>
       <c r="BT2" s="11" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="BU2" s="11" t="b">
         <v>0</v>
@@ -3776,196 +3648,196 @@
         <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="L3" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="N3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>183</v>
-      </c>
       <c r="Q3" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>251</v>
+        <v>196</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>85</v>
       </c>
       <c r="Y3" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="BD3" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="BE3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="BF3" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="BG3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="BI3" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="BK3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BL3" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="BM3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BN3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="BO3" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BP3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="BQ3" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="BR3" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="Z3" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL3" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AS3" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT3" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="AV3" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>264</v>
-      </c>
-      <c r="AX3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AY3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="BA3" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BB3" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="BE3" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BF3" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="BG3" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="BH3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BI3" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="BJ3" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="BK3" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL3" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="BM3" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BN3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BO3" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="BP3" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="BQ3" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BR3" s="4" t="s">
-        <v>246</v>
-      </c>
       <c r="BT3" s="11" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="BU3" s="11" t="b">
         <v>0</v>
@@ -3976,196 +3848,196 @@
         <v>81</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>309</v>
+        <v>246</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>269</v>
+        <v>208</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>281</v>
+        <v>218</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>269</v>
+        <v>208</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>285</v>
+        <v>222</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>286</v>
+        <v>223</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>287</v>
+        <v>224</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>288</v>
+        <v>225</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>289</v>
+        <v>226</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>290</v>
+        <v>227</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>291</v>
+        <v>228</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="AB4" s="6" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>292</v>
+        <v>229</v>
       </c>
       <c r="AD4" s="6" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
       <c r="AE4" s="6" t="s">
-        <v>294</v>
+        <v>231</v>
       </c>
       <c r="AF4" s="6" t="s">
-        <v>295</v>
+        <v>232</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="AH4" s="14" t="s">
-        <v>296</v>
+        <v>233</v>
       </c>
       <c r="AI4" s="14" t="s">
-        <v>297</v>
+        <v>234</v>
       </c>
       <c r="AJ4" s="6" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="AK4" s="14" t="s">
-        <v>296</v>
+        <v>233</v>
       </c>
       <c r="AL4" s="6" t="s">
-        <v>298</v>
+        <v>235</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>287</v>
+        <v>224</v>
       </c>
       <c r="AN4" s="6" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="AO4" t="s">
-        <v>300</v>
+        <v>237</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>299</v>
+        <v>236</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>279</v>
+        <v>216</v>
       </c>
       <c r="AW4" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
       <c r="AX4" s="4" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="AY4" s="4" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="AZ4" s="4" t="s">
-        <v>302</v>
+        <v>239</v>
       </c>
       <c r="BA4" s="6" t="s">
-        <v>303</v>
+        <v>240</v>
       </c>
       <c r="BB4" s="6" t="s">
-        <v>304</v>
+        <v>241</v>
       </c>
       <c r="BC4" s="6" t="s">
-        <v>303</v>
+        <v>240</v>
       </c>
       <c r="BD4" s="6" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="BE4" s="6" t="s">
-        <v>305</v>
+        <v>242</v>
       </c>
       <c r="BF4" s="4" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="BG4" s="4" t="s">
-        <v>306</v>
+        <v>243</v>
       </c>
       <c r="BH4" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="BI4" s="6" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="BJ4" s="4" t="s">
-        <v>294</v>
+        <v>231</v>
       </c>
       <c r="BK4" s="6" t="s">
-        <v>280</v>
+        <v>217</v>
       </c>
       <c r="BL4" s="4" t="s">
-        <v>294</v>
+        <v>231</v>
       </c>
       <c r="BM4" s="6" t="s">
-        <v>280</v>
+        <v>217</v>
       </c>
       <c r="BN4" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="BO4" s="4" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="BP4" s="4" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="BQ4" s="6" t="s">
-        <v>307</v>
+        <v>244</v>
       </c>
       <c r="BR4" s="4" t="s">
-        <v>308</v>
+        <v>245</v>
       </c>
       <c r="BT4" s="11" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="BU4" s="11" t="b">
         <v>0</v>
@@ -4176,13 +4048,13 @@
         <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>310</v>
+        <v>247</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>270</v>
+        <v>209</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>281</v>
+        <v>218</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -4211,7 +4083,7 @@
       <c r="BP5" s="4"/>
       <c r="BR5" s="4"/>
       <c r="BT5" s="11" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="BU5" s="11" t="b">
         <v>0</v>
@@ -4221,195 +4093,43 @@
       <c r="A6" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="D6" s="6" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE6" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="AC6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AO6"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BF6" s="4"/>
+      <c r="BG6" s="4"/>
+      <c r="BJ6" s="4"/>
+      <c r="BL6" s="4"/>
+      <c r="BO6" s="4"/>
+      <c r="BP6" s="4"/>
+      <c r="BR6" s="4"/>
+      <c r="BT6" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI6" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>210</v>
-      </c>
-      <c r="AS6" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT6" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU6" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="AV6" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>264</v>
-      </c>
-      <c r="AX6" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="AY6" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="BA6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BB6" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BD6" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="BE6" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BF6" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="BG6" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="BH6" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BI6" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="BJ6" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BK6" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL6" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="BM6" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BN6" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BO6" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="BP6" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="BQ6" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BR6" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="BT6" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="BU6" s="11" t="b">
         <v>0</v>
@@ -4419,195 +4139,45 @@
       <c r="A7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="D7" s="6" t="s">
-        <v>272</v>
+        <v>211</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="S7" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="T7" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH7" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI7" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="AK7" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM7" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN7" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>209</v>
-      </c>
-      <c r="AS7" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT7" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="AU7" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="AV7" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>264</v>
-      </c>
-      <c r="AX7" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="AY7" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="AZ7" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="BA7" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BB7" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC7" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BD7" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="BE7" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BF7" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="BG7" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="BH7" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BI7" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="BJ7" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="BK7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL7" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="BM7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="BN7" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="BO7" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="BP7" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="BQ7" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="BR7" s="4" t="s">
-        <v>248</v>
-      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="AC7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AO7"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
+      <c r="BF7" s="4"/>
+      <c r="BG7" s="4"/>
+      <c r="BJ7" s="4"/>
+      <c r="BL7" s="4"/>
+      <c r="BO7" s="4"/>
+      <c r="BP7" s="4"/>
+      <c r="BR7" s="4"/>
       <c r="BT7" s="11" t="s">
-        <v>263</v>
+        <v>204</v>
       </c>
       <c r="BU7" s="11" t="b">
         <v>0</v>
@@ -4623,10 +4193,184 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="29.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG1" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK1" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4649,106 +4393,106 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="I1" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="AH1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="AJ1" s="15" t="s">
         <v>11</v>
@@ -4759,47 +4503,47 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E2" s="15">
         <v>2710</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>259</v>
+        <v>200</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="O2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="L2" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>132</v>
-      </c>
       <c r="Q2" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="R2" s="15">
         <v>121212</v>
@@ -4809,10 +4553,10 @@
       </c>
       <c r="T2" s="15"/>
       <c r="U2" s="15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="V2" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
@@ -4820,13 +4564,13 @@
         <v>1434444</v>
       </c>
       <c r="Z2" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AB2" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AC2" s="15"/>
       <c r="AD2" s="15"/>
@@ -4844,51 +4588,51 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E3" s="15">
         <v>2710</v>
       </c>
       <c r="F3" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="O3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>132</v>
-      </c>
       <c r="Q3" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="R3" s="15">
         <v>121212</v>
@@ -4898,10 +4642,10 @@
       </c>
       <c r="T3" s="15"/>
       <c r="U3" s="15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="V3" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
@@ -4909,13 +4653,13 @@
         <v>1434444</v>
       </c>
       <c r="Z3" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AA3" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AC3" s="15"/>
       <c r="AD3" s="15"/>
@@ -4933,51 +4677,51 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>312</v>
+        <v>249</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E4" s="15">
         <v>2710</v>
       </c>
       <c r="F4" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="N4" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="O4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>132</v>
-      </c>
       <c r="Q4" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="R4" s="15">
         <v>121212</v>
@@ -4987,10 +4731,10 @@
       </c>
       <c r="T4" s="15"/>
       <c r="U4" s="15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="V4" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
@@ -4998,20 +4742,20 @@
         <v>1434444</v>
       </c>
       <c r="Z4" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AA4" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AB4" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AC4" s="15"/>
       <c r="AD4" s="15"/>
       <c r="AE4" s="15"/>
       <c r="AF4" s="15"/>
       <c r="AG4" s="15" t="s">
-        <v>313</v>
+        <v>250</v>
       </c>
       <c r="AH4" s="15"/>
       <c r="AI4" s="15"/>

</xml_diff>

<commit_message>
Added Test Case QA_TestCase_Auto_Optimus_2_2_1
Added Test Case QA_TestCase_Auto_Optimus_2_2_1
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FD6073-5FF8-44CB-965E-7E2A2BD0E381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="331">
   <si>
     <t>Username</t>
   </si>
@@ -840,13 +839,184 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_Optimus_3_1_4</t>
+  </si>
+  <si>
+    <t>Joe Pen QA</t>
+  </si>
+  <si>
+    <t>Fname TXA</t>
+  </si>
+  <si>
+    <t>Lname TXA</t>
+  </si>
+  <si>
+    <t>2002-08-03</t>
+  </si>
+  <si>
+    <t>2023-08-01 00:00:00</t>
+  </si>
+  <si>
+    <t>998877663322</t>
+  </si>
+  <si>
+    <t>Automation@txa.com</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>Shareholder</t>
+  </si>
+  <si>
+    <t>2022-09-07 07:00:00</t>
+  </si>
+  <si>
+    <t>2022-11-07 07:00:00</t>
+  </si>
+  <si>
+    <t>TXA1</t>
+  </si>
+  <si>
+    <t>TXA Automate FRN</t>
+  </si>
+  <si>
+    <t>TXA Automate CN</t>
+  </si>
+  <si>
+    <t>Institutional Fund</t>
+  </si>
+  <si>
+    <t>Business Registration</t>
+  </si>
+  <si>
+    <t>998877665544</t>
+  </si>
+  <si>
+    <t>Registered Address TXAutomate 1</t>
+  </si>
+  <si>
+    <t>OAddress TXA</t>
+  </si>
+  <si>
+    <t>Face to Face</t>
+  </si>
+  <si>
+    <t>SOFR TXAutomate</t>
+  </si>
+  <si>
+    <t>US TXA</t>
+  </si>
+  <si>
+    <t>SOWR TXA Automate</t>
+  </si>
+  <si>
+    <t>PBAR TXA Automate</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_2_2</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_2_3</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_2_4</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_2_5</t>
+  </si>
+  <si>
+    <t>Joe Pen QA2</t>
+  </si>
+  <si>
+    <t>LN Updt TXA</t>
+  </si>
+  <si>
+    <t>TXA U</t>
+  </si>
+  <si>
+    <t>2003-08-04</t>
+  </si>
+  <si>
+    <t>2022-07-01 00:00:01</t>
+  </si>
+  <si>
+    <t>2023-07-01 00:00:01</t>
+  </si>
+  <si>
+    <t>998877663311</t>
+  </si>
+  <si>
+    <t>AutomationUpdate@txa.com</t>
+  </si>
+  <si>
+    <t>Employment Income</t>
+  </si>
+  <si>
+    <t>SOFR TXAutomate Update</t>
+  </si>
+  <si>
+    <t>US TXA Upd</t>
+  </si>
+  <si>
+    <t>SOWR TXA Automate Updt</t>
+  </si>
+  <si>
+    <t>General Partner</t>
+  </si>
+  <si>
+    <t>TXA2</t>
+  </si>
+  <si>
+    <t>2022-10-07 07:00:01</t>
+  </si>
+  <si>
+    <t>2022-12-07 07:00:01</t>
+  </si>
+  <si>
+    <t>TXA Automate CN UPDT</t>
+  </si>
+  <si>
+    <t>TXA Automate FRN UPDT</t>
+  </si>
+  <si>
+    <t>Brokerage</t>
+  </si>
+  <si>
+    <t>Limited Partnership</t>
+  </si>
+  <si>
+    <t>998877665511</t>
+  </si>
+  <si>
+    <t>RA TXAutomate 2 Upd</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>OAddress TXA UPDT</t>
+  </si>
+  <si>
+    <t>Proprietary Trading</t>
+  </si>
+  <si>
+    <t>PBAR TXA Automate UPDT</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Token Sale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,13 +1046,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -993,11 +1176,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1009,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1051,21 +1234,199 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="115">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -2723,84 +3084,133 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="72">
-  <autoFilter ref="A1:BU7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="114">
+  <autoFilter ref="A1:BU7"/>
   <tableColumns count="73">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TestCaseID" dataDxfId="71"/>
-    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="ActionsTempField" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CounterparyRef" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NitroClientID" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SalesForceID" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ElwoodID" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NicknameExternal" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NicknameInternal" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ParentAccount" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FirstName" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="LastName" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nationality" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DateofBirth" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Occupation" dataDxfId="57"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CompanyofEmployment" dataDxfId="56"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IndustryofEmployment" dataDxfId="55"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IdentificationIssueDate" dataDxfId="54"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IdentificationExpiryDate" dataDxfId="53"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MobileNumber" dataDxfId="52"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PEPDeclaration" dataDxfId="51"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="PEPDeclarationRemarks" dataDxfId="50"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Alias" dataDxfId="49"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TIN1" dataDxfId="48"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TIN2" dataDxfId="47"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="TIN3" dataDxfId="46"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CompanyName" dataDxfId="45"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="FormerRegisteredName" dataDxfId="44"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ClientType" dataDxfId="43"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="EntityType" dataDxfId="42"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IdentificationNumber" dataDxfId="41"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="IdentificationType" dataDxfId="40"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="RegisteredAddress" dataDxfId="39"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="CountryofIncorporation" dataDxfId="38"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="StateofIncorporation" dataDxfId="37"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="OperatingAddress" dataDxfId="36"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="CountryofOperation" dataDxfId="35"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="OnboardingMode" dataDxfId="34"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="PrimaryBusinessActivity" dataDxfId="33"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="PrimaryBusinessActivityRemarks" dataDxfId="32"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="CorporateWebsite"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="GSTRegistered" dataDxfId="31"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="FinancialInstitution" dataDxfId="30"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PaymentServiceProvider" dataDxfId="29"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="SourceofFunds" dataDxfId="28"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="SourceofFundsRemarks" dataDxfId="27"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="AuthorizedPerson" dataDxfId="26"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="AuthorizedPersonMobile" dataDxfId="25"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="AuthorizedPersonEmail" dataDxfId="24"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="BusinessPurposeforRelationship" dataDxfId="23"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="AppointmentOthers" dataDxfId="22"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="GroupAssociation" dataDxfId="21"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="OnboardedDate" dataDxfId="20"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="ClientTier" dataDxfId="19"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="KYCRefreshDate" dataDxfId="18"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="ClientTierRemarks" dataDxfId="17"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RiskScore" dataDxfId="16"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RiskScoreRemarks" dataDxfId="15"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="ExecutionFeeRate" dataDxfId="14"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="ReferralPersonInternal" dataDxfId="13"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="ReferralPersonExternal" dataDxfId="12"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="ReferralExternalRebate" dataDxfId="11"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="FacetoFaceVerificationStatus" dataDxfId="10"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="FacetoFaceVerificationRemarks" dataDxfId="9"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="VouchedStatus" dataDxfId="8"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="VouchedbyPerson" dataDxfId="7"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="VouchedRemarks" dataDxfId="6"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="ManagementRemarks" dataDxfId="5"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="CounterpartyStatus" dataDxfId="4"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="CounterpartyRemarks" dataDxfId="3"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Messages" dataDxfId="2"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="SkipAtStepNum" dataDxfId="1"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="SIT" dataDxfId="0"/>
+    <tableColumn id="1" name="TestCaseID" dataDxfId="113"/>
+    <tableColumn id="73" name="ActionsTempField" dataDxfId="112"/>
+    <tableColumn id="2" name="CounterparyRef" dataDxfId="111"/>
+    <tableColumn id="3" name="NitroClientID" dataDxfId="110"/>
+    <tableColumn id="4" name="SalesForceID" dataDxfId="109"/>
+    <tableColumn id="5" name="ElwoodID" dataDxfId="108"/>
+    <tableColumn id="6" name="NicknameExternal" dataDxfId="107"/>
+    <tableColumn id="7" name="NicknameInternal" dataDxfId="106"/>
+    <tableColumn id="8" name="ParentAccount" dataDxfId="105"/>
+    <tableColumn id="9" name="FirstName" dataDxfId="104"/>
+    <tableColumn id="10" name="LastName" dataDxfId="103"/>
+    <tableColumn id="11" name="Gender" dataDxfId="102"/>
+    <tableColumn id="12" name="Nationality" dataDxfId="101"/>
+    <tableColumn id="13" name="DateofBirth" dataDxfId="100"/>
+    <tableColumn id="14" name="Occupation" dataDxfId="99"/>
+    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="98"/>
+    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="97"/>
+    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="96"/>
+    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="95"/>
+    <tableColumn id="19" name="MobileNumber" dataDxfId="94"/>
+    <tableColumn id="20" name="PEPDeclaration" dataDxfId="93"/>
+    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="92"/>
+    <tableColumn id="22" name="Alias" dataDxfId="91"/>
+    <tableColumn id="23" name="TIN1" dataDxfId="90"/>
+    <tableColumn id="24" name="TIN2" dataDxfId="89"/>
+    <tableColumn id="25" name="TIN3" dataDxfId="88"/>
+    <tableColumn id="26" name="CompanyName" dataDxfId="87"/>
+    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="86"/>
+    <tableColumn id="28" name="ClientType" dataDxfId="85"/>
+    <tableColumn id="29" name="EntityType" dataDxfId="84"/>
+    <tableColumn id="30" name="IdentificationNumber" dataDxfId="83"/>
+    <tableColumn id="31" name="IdentificationType" dataDxfId="82"/>
+    <tableColumn id="32" name="RegisteredAddress" dataDxfId="81"/>
+    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="80"/>
+    <tableColumn id="34" name="StateofIncorporation" dataDxfId="79"/>
+    <tableColumn id="35" name="OperatingAddress" dataDxfId="78"/>
+    <tableColumn id="36" name="CountryofOperation" dataDxfId="77"/>
+    <tableColumn id="37" name="OnboardingMode" dataDxfId="76"/>
+    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="75"/>
+    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="74"/>
+    <tableColumn id="40" name="CorporateWebsite"/>
+    <tableColumn id="41" name="GSTRegistered" dataDxfId="73"/>
+    <tableColumn id="42" name="FinancialInstitution" dataDxfId="72"/>
+    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="71"/>
+    <tableColumn id="44" name="SourceofFunds" dataDxfId="70"/>
+    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="69"/>
+    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="68"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="67"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="66"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="65"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="64"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="63"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="62"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="61"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="60"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="59"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="58"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="57"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="56"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="55"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="54"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="53"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="52"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="51"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="50"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="49"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="48"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="47"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="46"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="45"/>
+    <tableColumn id="70" name="Messages" dataDxfId="44"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="43"/>
+    <tableColumn id="72" name="SIT" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AN7" totalsRowShown="0" headerRowBorderDxfId="41" tableBorderDxfId="40">
+  <autoFilter ref="A1:AN7"/>
+  <tableColumns count="40">
+    <tableColumn id="1" name="TestCaseID" dataDxfId="39"/>
+    <tableColumn id="2" name="Action" dataDxfId="38"/>
+    <tableColumn id="3" name="RelatedPartyRef." dataDxfId="37"/>
+    <tableColumn id="4" name="Counterparty" dataDxfId="36"/>
+    <tableColumn id="5" name="FirstName" dataDxfId="35"/>
+    <tableColumn id="6" name="LastName" dataDxfId="34"/>
+    <tableColumn id="7" name="Gender" dataDxfId="33"/>
+    <tableColumn id="8" name="Nationality" dataDxfId="32"/>
+    <tableColumn id="9" name="DateOfBirth" dataDxfId="31"/>
+    <tableColumn id="10" name="IdentificationIssueDate" dataDxfId="30"/>
+    <tableColumn id="11" name="IdentificationExpiryDate" dataDxfId="29"/>
+    <tableColumn id="12" name="MobileNumber" dataDxfId="28"/>
+    <tableColumn id="13" name="EmailAddress" dataDxfId="27"/>
+    <tableColumn id="14" name="SourceOfFunds" dataDxfId="26"/>
+    <tableColumn id="15" name="SourceOfFundsRemarks" dataDxfId="25"/>
+    <tableColumn id="16" name="PEP" dataDxfId="24"/>
+    <tableColumn id="17" name="UltimateShareholding" dataDxfId="23"/>
+    <tableColumn id="18" name="SourceOfWealth" dataDxfId="22"/>
+    <tableColumn id="19" name="SourceOfWealthRemarks" dataDxfId="21"/>
+    <tableColumn id="20" name="Appointment" dataDxfId="20"/>
+    <tableColumn id="21" name="AppointmentAppointDate" dataDxfId="19"/>
+    <tableColumn id="22" name="AppointmentResignDate" dataDxfId="18"/>
+    <tableColumn id="23" name="Alias" dataDxfId="17"/>
+    <tableColumn id="24" name="CompanyName" dataDxfId="16"/>
+    <tableColumn id="25" name="FormerRegisteredName" dataDxfId="15"/>
+    <tableColumn id="26" name="ClientType" dataDxfId="14"/>
+    <tableColumn id="27" name="EntityType" dataDxfId="13"/>
+    <tableColumn id="28" name="IdentificationNumber" dataDxfId="12"/>
+    <tableColumn id="29" name="IdentificationType" dataDxfId="11"/>
+    <tableColumn id="30" name="RegisteredAddress" dataDxfId="10"/>
+    <tableColumn id="31" name="CountryOfIncorporation" dataDxfId="9"/>
+    <tableColumn id="32" name="StateOfIncorporation" dataDxfId="8"/>
+    <tableColumn id="33" name="OperationAddress" dataDxfId="7"/>
+    <tableColumn id="34" name="CountryOfOperation" dataDxfId="6"/>
+    <tableColumn id="35" name="OnboardingMode" dataDxfId="5"/>
+    <tableColumn id="36" name="PrimaryBusinessActivity" dataDxfId="4"/>
+    <tableColumn id="37" name="PrimaryBusinessActivityRemarks" dataDxfId="3"/>
+    <tableColumn id="38" name="Messages" dataDxfId="2"/>
+    <tableColumn id="39" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="40" name="SIT" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2880,23 +3290,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2932,23 +3325,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3124,7 +3500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3251,9 +3627,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -3261,10 +3637,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3564,7 +3942,9 @@
       </c>
     </row>
     <row r="2" spans="1:73" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16"/>
+      <c r="A2" s="16" t="s">
+        <v>329</v>
+      </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -4231,185 +4611,526 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="32.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="29.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AA1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AB1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AC1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AD1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AF1" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AG1" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AH1" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="AJ1" s="19" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AK1" s="19" t="s">
+      <c r="AK1" s="21" t="s">
         <v>48</v>
       </c>
+      <c r="AL1" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN1" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AE2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ2" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="17"/>
+      <c r="AM2" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN2" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>213</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="M3" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="AH3" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="AJ3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK3" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="AL3" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="AM3" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN3" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="M4" t="s">
+        <v>310</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD4" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF4" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="AH4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI4" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ4" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="AK4" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="AL4" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="AM4" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN4" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="AM5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN5" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="AM6" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN6" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="AM7" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN7" s="18" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
QA_TestCase_Auto_Optimus_2_2_2 - 3 and 4
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F4EC9-8DCB-4396-A451-9ED26761917A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
@@ -19,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="385">
   <si>
     <t>Username</t>
   </si>
@@ -1171,12 +1170,15 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_Optimus_4_1_3</t>
+  </si>
+  <si>
+    <t>Download Btn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3263,131 +3265,131 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="114">
-  <autoFilter ref="A1:BU7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BU7" totalsRowShown="0" tableBorderDxfId="114">
+  <autoFilter ref="A1:BU7"/>
   <tableColumns count="73">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TestCaseID" dataDxfId="113"/>
-    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="ActionsTempField" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CounterparyRef" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NitroClientID" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SalesForceID" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ElwoodID" dataDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NicknameExternal" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NicknameInternal" dataDxfId="106"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ParentAccount" dataDxfId="105"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FirstName" dataDxfId="104"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="LastName" dataDxfId="103"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="102"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nationality" dataDxfId="101"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DateofBirth" dataDxfId="100"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Occupation" dataDxfId="99"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CompanyofEmployment" dataDxfId="98"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IndustryofEmployment" dataDxfId="97"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IdentificationIssueDate" dataDxfId="96"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IdentificationExpiryDate" dataDxfId="95"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MobileNumber" dataDxfId="94"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PEPDeclaration" dataDxfId="93"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="PEPDeclarationRemarks" dataDxfId="92"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Alias" dataDxfId="91"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TIN1" dataDxfId="90"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TIN2" dataDxfId="89"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="TIN3" dataDxfId="88"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CompanyName" dataDxfId="87"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="FormerRegisteredName" dataDxfId="86"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ClientType" dataDxfId="85"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="EntityType" dataDxfId="84"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IdentificationNumber" dataDxfId="83"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="IdentificationType" dataDxfId="82"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="RegisteredAddress" dataDxfId="81"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="CountryofIncorporation" dataDxfId="80"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="StateofIncorporation" dataDxfId="79"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="OperatingAddress" dataDxfId="78"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="CountryofOperation" dataDxfId="77"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="OnboardingMode" dataDxfId="76"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="PrimaryBusinessActivity" dataDxfId="75"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="PrimaryBusinessActivityRemarks" dataDxfId="74"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="CorporateWebsite"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="GSTRegistered" dataDxfId="73"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="FinancialInstitution" dataDxfId="72"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="PaymentServiceProvider" dataDxfId="71"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="SourceofFunds" dataDxfId="70"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="SourceofFundsRemarks" dataDxfId="69"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="AuthorizedPerson" dataDxfId="68"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="AuthorizedPersonMobile" dataDxfId="67"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="AuthorizedPersonEmail" dataDxfId="66"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="BusinessPurposeforRelationship" dataDxfId="65"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="AppointmentOthers" dataDxfId="64"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="GroupAssociation" dataDxfId="63"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="OnboardedDate" dataDxfId="62"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="ClientTier" dataDxfId="61"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="KYCRefreshDate" dataDxfId="60"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="ClientTierRemarks" dataDxfId="59"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="RiskScore" dataDxfId="58"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="RiskScoreRemarks" dataDxfId="57"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="ExecutionFeeRate" dataDxfId="56"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="ReferralPersonInternal" dataDxfId="55"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="ReferralPersonExternal" dataDxfId="54"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="ReferralExternalRebate" dataDxfId="53"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="FacetoFaceVerificationStatus" dataDxfId="52"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="FacetoFaceVerificationRemarks" dataDxfId="51"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="VouchedStatus" dataDxfId="50"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="VouchedbyPerson" dataDxfId="49"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="VouchedRemarks" dataDxfId="48"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="ManagementRemarks" dataDxfId="47"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="CounterpartyStatus" dataDxfId="46"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="CounterpartyRemarks" dataDxfId="45"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Messages" dataDxfId="44"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="SkipAtStepNum" dataDxfId="43"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="SIT" dataDxfId="42"/>
+    <tableColumn id="1" name="TestCaseID" dataDxfId="113"/>
+    <tableColumn id="73" name="ActionsTempField" dataDxfId="112"/>
+    <tableColumn id="2" name="CounterparyRef" dataDxfId="111"/>
+    <tableColumn id="3" name="NitroClientID" dataDxfId="110"/>
+    <tableColumn id="4" name="SalesForceID" dataDxfId="109"/>
+    <tableColumn id="5" name="ElwoodID" dataDxfId="108"/>
+    <tableColumn id="6" name="NicknameExternal" dataDxfId="107"/>
+    <tableColumn id="7" name="NicknameInternal" dataDxfId="106"/>
+    <tableColumn id="8" name="ParentAccount" dataDxfId="105"/>
+    <tableColumn id="9" name="FirstName" dataDxfId="104"/>
+    <tableColumn id="10" name="LastName" dataDxfId="103"/>
+    <tableColumn id="11" name="Gender" dataDxfId="102"/>
+    <tableColumn id="12" name="Nationality" dataDxfId="101"/>
+    <tableColumn id="13" name="DateofBirth" dataDxfId="100"/>
+    <tableColumn id="14" name="Occupation" dataDxfId="99"/>
+    <tableColumn id="15" name="CompanyofEmployment" dataDxfId="98"/>
+    <tableColumn id="16" name="IndustryofEmployment" dataDxfId="97"/>
+    <tableColumn id="17" name="IdentificationIssueDate" dataDxfId="96"/>
+    <tableColumn id="18" name="IdentificationExpiryDate" dataDxfId="95"/>
+    <tableColumn id="19" name="MobileNumber" dataDxfId="94"/>
+    <tableColumn id="20" name="PEPDeclaration" dataDxfId="93"/>
+    <tableColumn id="21" name="PEPDeclarationRemarks" dataDxfId="92"/>
+    <tableColumn id="22" name="Alias" dataDxfId="91"/>
+    <tableColumn id="23" name="TIN1" dataDxfId="90"/>
+    <tableColumn id="24" name="TIN2" dataDxfId="89"/>
+    <tableColumn id="25" name="TIN3" dataDxfId="88"/>
+    <tableColumn id="26" name="CompanyName" dataDxfId="87"/>
+    <tableColumn id="27" name="FormerRegisteredName" dataDxfId="86"/>
+    <tableColumn id="28" name="ClientType" dataDxfId="85"/>
+    <tableColumn id="29" name="EntityType" dataDxfId="84"/>
+    <tableColumn id="30" name="IdentificationNumber" dataDxfId="83"/>
+    <tableColumn id="31" name="IdentificationType" dataDxfId="82"/>
+    <tableColumn id="32" name="RegisteredAddress" dataDxfId="81"/>
+    <tableColumn id="33" name="CountryofIncorporation" dataDxfId="80"/>
+    <tableColumn id="34" name="StateofIncorporation" dataDxfId="79"/>
+    <tableColumn id="35" name="OperatingAddress" dataDxfId="78"/>
+    <tableColumn id="36" name="CountryofOperation" dataDxfId="77"/>
+    <tableColumn id="37" name="OnboardingMode" dataDxfId="76"/>
+    <tableColumn id="38" name="PrimaryBusinessActivity" dataDxfId="75"/>
+    <tableColumn id="39" name="PrimaryBusinessActivityRemarks" dataDxfId="74"/>
+    <tableColumn id="40" name="CorporateWebsite"/>
+    <tableColumn id="41" name="GSTRegistered" dataDxfId="73"/>
+    <tableColumn id="42" name="FinancialInstitution" dataDxfId="72"/>
+    <tableColumn id="43" name="PaymentServiceProvider" dataDxfId="71"/>
+    <tableColumn id="44" name="SourceofFunds" dataDxfId="70"/>
+    <tableColumn id="45" name="SourceofFundsRemarks" dataDxfId="69"/>
+    <tableColumn id="46" name="AuthorizedPerson" dataDxfId="68"/>
+    <tableColumn id="47" name="AuthorizedPersonMobile" dataDxfId="67"/>
+    <tableColumn id="48" name="AuthorizedPersonEmail" dataDxfId="66"/>
+    <tableColumn id="49" name="BusinessPurposeforRelationship" dataDxfId="65"/>
+    <tableColumn id="50" name="AppointmentOthers" dataDxfId="64"/>
+    <tableColumn id="51" name="GroupAssociation" dataDxfId="63"/>
+    <tableColumn id="52" name="OnboardedDate" dataDxfId="62"/>
+    <tableColumn id="53" name="ClientTier" dataDxfId="61"/>
+    <tableColumn id="54" name="KYCRefreshDate" dataDxfId="60"/>
+    <tableColumn id="55" name="ClientTierRemarks" dataDxfId="59"/>
+    <tableColumn id="56" name="RiskScore" dataDxfId="58"/>
+    <tableColumn id="57" name="RiskScoreRemarks" dataDxfId="57"/>
+    <tableColumn id="58" name="ExecutionFeeRate" dataDxfId="56"/>
+    <tableColumn id="59" name="ReferralPersonInternal" dataDxfId="55"/>
+    <tableColumn id="60" name="ReferralPersonExternal" dataDxfId="54"/>
+    <tableColumn id="61" name="ReferralExternalRebate" dataDxfId="53"/>
+    <tableColumn id="62" name="FacetoFaceVerificationStatus" dataDxfId="52"/>
+    <tableColumn id="63" name="FacetoFaceVerificationRemarks" dataDxfId="51"/>
+    <tableColumn id="64" name="VouchedStatus" dataDxfId="50"/>
+    <tableColumn id="65" name="VouchedbyPerson" dataDxfId="49"/>
+    <tableColumn id="66" name="VouchedRemarks" dataDxfId="48"/>
+    <tableColumn id="67" name="ManagementRemarks" dataDxfId="47"/>
+    <tableColumn id="68" name="CounterpartyStatus" dataDxfId="46"/>
+    <tableColumn id="69" name="CounterpartyRemarks" dataDxfId="45"/>
+    <tableColumn id="70" name="Messages" dataDxfId="44"/>
+    <tableColumn id="71" name="SkipAtStepNum" dataDxfId="43"/>
+    <tableColumn id="72" name="SIT" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:AN7" totalsRowShown="0" headerRowBorderDxfId="41" tableBorderDxfId="40">
-  <autoFilter ref="A1:AN7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AN7" totalsRowShown="0" headerRowBorderDxfId="41" tableBorderDxfId="40">
+  <autoFilter ref="A1:AN7"/>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TestCaseID" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Action" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="RelatedPartyRef." dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Counterparty" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="FirstName" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="LastName" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Gender" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Nationality" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="DateOfBirth" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="IdentificationIssueDate" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="IdentificationExpiryDate" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="MobileNumber" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="EmailAddress" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="SourceOfFunds" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="SourceOfFundsRemarks" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="PEP" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UltimateShareholding" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="SourceOfWealth" dataDxfId="22"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="SourceOfWealthRemarks" dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Appointment" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="AppointmentAppointDate" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="AppointmentResignDate" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Alias" dataDxfId="17"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="CompanyName" dataDxfId="16"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="FormerRegisteredName" dataDxfId="15"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="ClientType" dataDxfId="14"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="EntityType" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IdentificationNumber" dataDxfId="12"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IdentificationType" dataDxfId="11"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="RegisteredAddress" dataDxfId="10"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="CountryOfIncorporation" dataDxfId="9"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="StateOfIncorporation" dataDxfId="8"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="OperationAddress" dataDxfId="7"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="CountryOfOperation" dataDxfId="6"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="OnboardingMode" dataDxfId="5"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="PrimaryBusinessActivity" dataDxfId="4"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="PrimaryBusinessActivityRemarks" dataDxfId="3"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="Messages" dataDxfId="2"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="SkipAtStepNum" dataDxfId="1"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="SIT" dataDxfId="0"/>
+    <tableColumn id="1" name="TestCaseID" dataDxfId="39"/>
+    <tableColumn id="2" name="Action" dataDxfId="38"/>
+    <tableColumn id="3" name="RelatedPartyRef." dataDxfId="37"/>
+    <tableColumn id="4" name="Counterparty" dataDxfId="36"/>
+    <tableColumn id="5" name="FirstName" dataDxfId="35"/>
+    <tableColumn id="6" name="LastName" dataDxfId="34"/>
+    <tableColumn id="7" name="Gender" dataDxfId="33"/>
+    <tableColumn id="8" name="Nationality" dataDxfId="32"/>
+    <tableColumn id="9" name="DateOfBirth" dataDxfId="31"/>
+    <tableColumn id="10" name="IdentificationIssueDate" dataDxfId="30"/>
+    <tableColumn id="11" name="IdentificationExpiryDate" dataDxfId="29"/>
+    <tableColumn id="12" name="MobileNumber" dataDxfId="28"/>
+    <tableColumn id="13" name="EmailAddress" dataDxfId="27"/>
+    <tableColumn id="14" name="SourceOfFunds" dataDxfId="26"/>
+    <tableColumn id="15" name="SourceOfFundsRemarks" dataDxfId="25"/>
+    <tableColumn id="16" name="PEP" dataDxfId="24"/>
+    <tableColumn id="17" name="UltimateShareholding" dataDxfId="23"/>
+    <tableColumn id="18" name="SourceOfWealth" dataDxfId="22"/>
+    <tableColumn id="19" name="SourceOfWealthRemarks" dataDxfId="21"/>
+    <tableColumn id="20" name="Appointment" dataDxfId="20"/>
+    <tableColumn id="21" name="AppointmentAppointDate" dataDxfId="19"/>
+    <tableColumn id="22" name="AppointmentResignDate" dataDxfId="18"/>
+    <tableColumn id="23" name="Alias" dataDxfId="17"/>
+    <tableColumn id="24" name="CompanyName" dataDxfId="16"/>
+    <tableColumn id="25" name="FormerRegisteredName" dataDxfId="15"/>
+    <tableColumn id="26" name="ClientType" dataDxfId="14"/>
+    <tableColumn id="27" name="EntityType" dataDxfId="13"/>
+    <tableColumn id="28" name="IdentificationNumber" dataDxfId="12"/>
+    <tableColumn id="29" name="IdentificationType" dataDxfId="11"/>
+    <tableColumn id="30" name="RegisteredAddress" dataDxfId="10"/>
+    <tableColumn id="31" name="CountryOfIncorporation" dataDxfId="9"/>
+    <tableColumn id="32" name="StateOfIncorporation" dataDxfId="8"/>
+    <tableColumn id="33" name="OperationAddress" dataDxfId="7"/>
+    <tableColumn id="34" name="CountryOfOperation" dataDxfId="6"/>
+    <tableColumn id="35" name="OnboardingMode" dataDxfId="5"/>
+    <tableColumn id="36" name="PrimaryBusinessActivity" dataDxfId="4"/>
+    <tableColumn id="37" name="PrimaryBusinessActivityRemarks" dataDxfId="3"/>
+    <tableColumn id="38" name="Messages" dataDxfId="2"/>
+    <tableColumn id="39" name="SkipAtStepNum" dataDxfId="1"/>
+    <tableColumn id="40" name="SIT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3469,23 +3471,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3521,23 +3506,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3713,7 +3681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3840,9 +3808,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://system.qa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -3850,7 +3818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4824,11 +4792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5190,6 +5158,9 @@
       <c r="D4" s="11" t="s">
         <v>303</v>
       </c>
+      <c r="E4" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="F4" s="11" t="s">
         <v>304</v>
       </c>
@@ -5300,6 +5271,18 @@
       <c r="B5" s="11" t="s">
         <v>247</v>
       </c>
+      <c r="D5" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>253</v>
+      </c>
       <c r="AM5" s="18" t="s">
         <v>204</v>
       </c>
@@ -5311,6 +5294,21 @@
       <c r="A6" s="11" t="s">
         <v>301</v>
       </c>
+      <c r="B6" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>253</v>
+      </c>
       <c r="AM6" s="18" t="s">
         <v>204</v>
       </c>
@@ -5321,6 +5319,21 @@
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>302</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="AM7" s="18" t="s">
         <v>204</v>
@@ -5339,7 +5352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5836,11 +5849,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D0EAB0-328F-473A-85E4-0D7AD6F8940F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Optimus test data file
Updated Optimus test data file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Optimus.xlsx
+++ b/src/test/resources/testData/Optimus.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OptimusLogin" sheetId="9" r:id="rId1"/>
     <sheet name="CreateCounterParty" sheetId="11" r:id="rId2"/>
     <sheet name="RelatedCounterParty" sheetId="13" r:id="rId3"/>
-    <sheet name="Settlement" sheetId="12" r:id="rId4"/>
-    <sheet name="Portfolio" sheetId="14" r:id="rId5"/>
+    <sheet name="ServicesCounterParty" sheetId="15" r:id="rId4"/>
+    <sheet name="Settlement" sheetId="12" r:id="rId5"/>
+    <sheet name="Portfolio" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="415">
   <si>
     <t>Username</t>
   </si>
@@ -1173,6 +1174,96 @@
   </si>
   <si>
     <t>Download Btn</t>
+  </si>
+  <si>
+    <t>ServiceRef</t>
+  </si>
+  <si>
+    <t>BusinessUnit</t>
+  </si>
+  <si>
+    <t>ServiceName</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>ServiceTier</t>
+  </si>
+  <si>
+    <t>FeeRate</t>
+  </si>
+  <si>
+    <t>FeeType</t>
+  </si>
+  <si>
+    <t>ChargeRate</t>
+  </si>
+  <si>
+    <t>ChargeType</t>
+  </si>
+  <si>
+    <t>ServiceEntity</t>
+  </si>
+  <si>
+    <t>ServiceStatus</t>
+  </si>
+  <si>
+    <t>ServiceSignerName</t>
+  </si>
+  <si>
+    <t>ServiceStartDate</t>
+  </si>
+  <si>
+    <t>ServiceEndDate</t>
+  </si>
+  <si>
+    <t>ServiceContactPerson</t>
+  </si>
+  <si>
+    <t>ServiceContactPersonEmail</t>
+  </si>
+  <si>
+    <t>ServiceContactPersonMobile</t>
+  </si>
+  <si>
+    <t>ExpectedTradingVolume</t>
+  </si>
+  <si>
+    <t>MiningServiceTransferFee</t>
+  </si>
+  <si>
+    <t>MiningServiceHashrate</t>
+  </si>
+  <si>
+    <t>MiningServicePower</t>
+  </si>
+  <si>
+    <t>MiningServicePowerCharge</t>
+  </si>
+  <si>
+    <t>ReferralPerson</t>
+  </si>
+  <si>
+    <t>ServiceRemarks</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_3_1</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_3_2</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_3_3</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_3_4</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_Optimus_2_3_5</t>
+  </si>
+  <si>
+    <t>Edit</t>
   </si>
 </sst>
 </file>
@@ -4795,8 +4886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5353,6 +5444,191 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G1" t="s">
+        <v>388</v>
+      </c>
+      <c r="H1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J1" t="s">
+        <v>391</v>
+      </c>
+      <c r="K1" t="s">
+        <v>392</v>
+      </c>
+      <c r="L1" t="s">
+        <v>393</v>
+      </c>
+      <c r="M1" t="s">
+        <v>394</v>
+      </c>
+      <c r="N1" t="s">
+        <v>395</v>
+      </c>
+      <c r="O1" t="s">
+        <v>396</v>
+      </c>
+      <c r="P1" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>398</v>
+      </c>
+      <c r="R1" t="s">
+        <v>399</v>
+      </c>
+      <c r="S1" t="s">
+        <v>400</v>
+      </c>
+      <c r="T1" t="s">
+        <v>401</v>
+      </c>
+      <c r="U1" t="s">
+        <v>402</v>
+      </c>
+      <c r="V1" t="s">
+        <v>403</v>
+      </c>
+      <c r="W1" t="s">
+        <v>404</v>
+      </c>
+      <c r="X1" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>407</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>408</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>413</v>
+      </c>
+      <c r="B7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5848,7 +6124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>

</xml_diff>